<commit_message>
autofind the approximate xy centers
</commit_message>
<xml_diff>
--- a/mSPAGHETI_analysis_log_2014b.xlsx
+++ b/mSPAGHETI_analysis_log_2014b.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36660" yWindow="1000" windowWidth="35900" windowHeight="20400" tabRatio="500"/>
+    <workbookView xWindow="-36160" yWindow="600" windowWidth="35900" windowHeight="20400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" r:id="rId1"/>
@@ -19,20 +19,148 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="206">
+  <si>
+    <t>JHK_JPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>photomask200um</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130830/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub_area</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Directory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Basename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acq_Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d_mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_missing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_nonstandard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_mirror</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?838</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131202/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131014/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Desc:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mSPAGHETI log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flags…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Part</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>xc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>yc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Directory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -41,6 +169,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>°</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -49,65 +185,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/MIT/UTN18/20110131/</t>
-  </si>
-  <si>
-    <t>Project</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>utn18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>utn18_f838_L632_d15mm-</t>
-  </si>
-  <si>
-    <t>JPL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E09</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110509/</t>
-  </si>
-  <si>
-    <t>E09_R3_d25mm_f838mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110510/</t>
-  </si>
-  <si>
-    <t>E09_m0_d20mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dithered, see notes in .ppt document</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All data present, "G" instead of "D" as suffix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Flags…</t>
+    <t>pix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heritage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing most of the data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iSHELL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100624/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JWST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A6I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?632.8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -125,15 +247,141 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sub_area</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Acq_Date</t>
+    <t>E10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPL01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A100um</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mirror</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dithered</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>utn18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All data present</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_J/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ07_C_6mm_f200mm_632nm_sat_filt-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ07_D_6mm_f200mm_632nm_sat_filt-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a few saturated and unsaturated frames</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All data present, "G" instead of "D" as suffix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JHK_JPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/MIT/UTN18/20110131/</t>
+  </si>
+  <si>
+    <t>utn18_f838_L632_d15mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110509/</t>
+  </si>
+  <si>
+    <t>E09_R3_d25mm_f838mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110510/</t>
+  </si>
+  <si>
+    <t>E09_m0_d20mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dithered, see notes in .ppt document</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -141,27 +389,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_missing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_nonstandard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_mirror</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d_mm</t>
+    <t>;Author:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gully</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Date:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -177,69 +413,21 @@
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_E/</t>
   </si>
   <si>
-    <t>FL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20110930/</t>
   </si>
   <si>
     <t>E12_D25mm_f2m_l632nm_R3-</t>
   </si>
   <si>
-    <t>Note</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JPL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Missing most of the data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101028/</t>
   </si>
   <si>
     <t>JPL01_A100um_D12_5mm_L632nm_F838mm-</t>
   </si>
   <si>
-    <t>JPL01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mir_D12_5mm_L632nm_F838mm_dith-</t>
   </si>
   <si>
-    <t>A100um</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101102/</t>
   </si>
   <si>
@@ -249,10 +437,6 @@
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/mir/</t>
   </si>
   <si>
-    <t>mirror</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mir_D12_5mm_L632nm_F838mm-</t>
   </si>
   <si>
@@ -262,24 +446,12 @@
     <t>TJ02B_D12_5mm_L632nm_F838mm-</t>
   </si>
   <si>
-    <t>TJ02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101107/</t>
   </si>
   <si>
     <t>TJ02A_D12_5mm_L632nm_F838mm-</t>
   </si>
   <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110211/</t>
   </si>
   <si>
@@ -289,10 +461,6 @@
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213/</t>
   </si>
   <si>
-    <t>TJ03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TJ03A_blaze_d8_2mm_l632nm-</t>
   </si>
   <si>
@@ -302,71 +470,15 @@
     <t>TJ03C_blaze_d8_2mm_l632nm-</t>
   </si>
   <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_D/</t>
   </si>
   <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TJ03D_blaze_d8_2mm_l632nm-</t>
   </si>
   <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_F/</t>
   </si>
   <si>
-    <t>;Desc:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mSPAGHETI log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Author:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gully</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Date:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Part</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Basename</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D/</t>
   </si>
   <si>
@@ -376,22 +488,6 @@
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D_f200mm/</t>
   </si>
   <si>
-    <t>TJ07_C_6mm_f200mm_632nm_sat_filt-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ07_D_6mm_f200mm_632nm_sat_filt-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heritage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100217/</t>
   </si>
   <si>
@@ -401,24 +497,12 @@
     <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100220/</t>
   </si>
   <si>
-    <t>Heritage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>G1_L543nm_f400mm_d15mm_R2-</t>
   </si>
   <si>
     <t>E06_632nm_25mm_2000mm_hdr-</t>
   </si>
   <si>
-    <t>iSHELL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TJ03F_blaze_d8_2mm_l632nm_FL200mm-</t>
   </si>
   <si>
@@ -450,10 +534,6 @@
     <t>TJ03H_blaze_d8_2mm_l632nm_FL200mm-</t>
   </si>
   <si>
-    <t>TJ03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110215/</t>
   </si>
   <si>
@@ -463,10 +543,6 @@
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110217_mir/</t>
   </si>
   <si>
-    <t>mirror</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mirror_d8_2mm_l632nm_FL200mm-</t>
   </si>
   <si>
@@ -476,14 +552,6 @@
     <t>TJ04_25um_G_blaze_d8_2mm_l632nm_FL200mm-</t>
   </si>
   <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_H/</t>
   </si>
   <si>
@@ -498,10 +566,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_I/</t>
   </si>
   <si>
@@ -520,122 +584,51 @@
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_B/</t>
   </si>
   <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_J/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TJ04_100um_B_blaze_d8_2mm_l632nm_FL838mm-</t>
   </si>
   <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_C/</t>
   </si>
   <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131014</t>
-  </si>
-  <si>
     <t>E09_R3_d15mm_L632_f838-</t>
   </si>
   <si>
-    <t>?838</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>E12_R3_d15mm_L632_f838-</t>
   </si>
   <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100626/</t>
   </si>
   <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100624/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>E06_632nm_20mm_838mm_hdr-</t>
   </si>
   <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/E10/E10/</t>
   </si>
   <si>
-    <t>E10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>E10_20mm_632nm_838mm_R3-</t>
   </si>
   <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/E11/20110613/</t>
   </si>
   <si>
-    <t>E11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>E11_R3_d25mm_f838mm_632nm-</t>
   </si>
   <si>
-    <t>All data present</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All data present</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dithered</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a few saturated and unsaturated frames</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/20110111/</t>
   </si>
   <si>
     <t>g02_angle_pos1_dither1-</t>
   </si>
   <si>
-    <t>G02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pos1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pos2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>g02_angle_pos2_dither1-</t>
   </si>
   <si>
-    <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>iSHELL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/G02_optical/</t>
   </si>
   <si>
     <t>G02_R3_d15mm_w632nm_f838mm-</t>
   </si>
   <si>
-    <t>G03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G03/</t>
   </si>
   <si>
@@ -651,10 +644,6 @@
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A/</t>
   </si>
   <si>
-    <t>TJ07</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TJ07_A_d6mm_f838mm_632nm-</t>
   </si>
   <si>
@@ -685,60 +674,33 @@
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C_f200mm/</t>
   </si>
   <si>
-    <t>?632.8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131016/</t>
   </si>
   <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20131108/</t>
   </si>
   <si>
-    <t>mirror</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mirror_d15mm_L632_f838-</t>
   </si>
   <si>
-    <t>?15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>JHKishell_d5mm_L632_f838-</t>
   </si>
   <si>
     <t>Mirror_d5mm_L632_f838-</t>
   </si>
   <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>JHKishell_d5mm_L632_f838_B-</t>
   </si>
   <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131203</t>
   </si>
   <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131202</t>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20140113/SIGRTUTIShell_JHK_B</t>
   </si>
   <si>
-    <t>;#</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>G03_R3_d25mm_L632_f838-</t>
   </si>
   <si>
-    <t>G05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G05/</t>
   </si>
   <si>
@@ -748,17 +710,9 @@
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130628_mir/</t>
   </si>
   <si>
-    <t>mirror</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mir_d25mm_L632_f838-</t>
   </si>
   <si>
-    <t>JHK_JPL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130423_ishell_JHK/</t>
   </si>
   <si>
@@ -780,53 +734,26 @@
     <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130827_mir/</t>
   </si>
   <si>
-    <t>JWST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/sim_grate/A6I_scattered/scattered/</t>
   </si>
   <si>
-    <t>A6I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>scattered-</t>
   </si>
   <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130830/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mask200um_top10um_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>photomask200um</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -887,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -909,10 +836,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1244,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1253,15 +1181,15 @@
     <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" style="1"/>
     <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
     <col min="6" max="6" width="40.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="1" customWidth="1"/>
     <col min="9" max="10" width="5.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" customWidth="1"/>
     <col min="12" max="12" width="4.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="3.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="3.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" style="1" customWidth="1"/>
     <col min="15" max="15" width="19.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="6.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="9.28515625" style="1" customWidth="1"/>
@@ -1271,15 +1199,15 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B2" s="2">
         <v>40190</v>
@@ -1287,137 +1215,137 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="N7" s="4" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>33</v>
+        <v>13</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="6" t="s">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="J8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="M8" s="8" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1425,19 +1353,19 @@
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="G10" s="5">
         <v>20100217</v>
@@ -1458,8 +1386,14 @@
       <c r="L10" s="1">
         <v>512</v>
       </c>
+      <c r="M10" s="17">
+        <v>421.19099999999997</v>
+      </c>
+      <c r="N10" s="17">
+        <v>445.50299999999999</v>
+      </c>
       <c r="O10" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P10" s="1">
         <v>1</v>
@@ -1476,19 +1410,19 @@
         <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="G11" s="5">
         <v>20100220</v>
@@ -1509,8 +1443,14 @@
       <c r="L11" s="1">
         <v>400</v>
       </c>
+      <c r="M11" s="17">
+        <v>476.17</v>
+      </c>
+      <c r="N11" s="17">
+        <v>485.83199999999999</v>
+      </c>
       <c r="O11" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P11" s="1">
         <v>1</v>
@@ -1527,19 +1467,19 @@
         <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>145</v>
+        <v>47</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="G12" s="5">
         <v>20100624</v>
@@ -1560,8 +1500,14 @@
       <c r="L12" s="1">
         <v>256</v>
       </c>
+      <c r="M12" s="17">
+        <v>513.56500000000005</v>
+      </c>
+      <c r="N12" s="17">
+        <v>431.52600000000001</v>
+      </c>
       <c r="O12" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P12" s="1">
         <v>1</v>
@@ -1578,19 +1524,19 @@
         <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>146</v>
+        <v>46</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="G13" s="5">
         <v>20100626</v>
@@ -1611,8 +1557,14 @@
       <c r="L13" s="1">
         <v>256</v>
       </c>
+      <c r="M13" s="17">
+        <v>815.22400000000005</v>
+      </c>
+      <c r="N13" s="17">
+        <v>291.541</v>
+      </c>
       <c r="O13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P13" s="1">
         <v>1</v>
@@ -1629,19 +1581,19 @@
         <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G14" s="1">
         <v>20100719</v>
@@ -1662,8 +1614,14 @@
       <c r="L14" s="1">
         <v>256</v>
       </c>
+      <c r="M14" s="17">
+        <v>631.07399999999996</v>
+      </c>
+      <c r="N14" s="17">
+        <v>426.42599999999999</v>
+      </c>
       <c r="O14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P14" s="1">
         <v>1</v>
@@ -1680,40 +1638,46 @@
         <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>215</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>217</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G15" s="1">
         <v>20100817</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>191</v>
+        <v>51</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>186</v>
+        <v>52</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>142</v>
+        <v>18</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="L15" s="1">
         <v>500</v>
       </c>
+      <c r="M15" s="17">
+        <v>724.15200000000004</v>
+      </c>
+      <c r="N15" s="17">
+        <v>707.85699999999997</v>
+      </c>
       <c r="O15" s="12" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
@@ -1730,19 +1694,19 @@
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>149</v>
+        <v>54</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="G16" s="5">
         <v>20100824</v>
@@ -1763,8 +1727,14 @@
       <c r="L16" s="1">
         <v>256</v>
       </c>
+      <c r="M16" s="17">
+        <v>534.60199999999998</v>
+      </c>
+      <c r="N16" s="17">
+        <v>390.601</v>
+      </c>
       <c r="O16" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P16" s="1">
         <v>1</v>
@@ -1781,19 +1751,19 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="G17" s="5">
         <v>20101028</v>
@@ -1813,8 +1783,14 @@
       <c r="L17" s="1">
         <v>256</v>
       </c>
+      <c r="M17" s="17">
+        <v>855.43399999999997</v>
+      </c>
+      <c r="N17" s="17">
+        <v>691.86699999999996</v>
+      </c>
       <c r="O17" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P17" s="1">
         <v>1</v>
@@ -1831,19 +1807,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="G18" s="5">
         <v>20101028</v>
@@ -1863,14 +1839,14 @@
       <c r="L18" s="1">
         <v>15</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>91</v>
+      <c r="M18" s="17">
+        <v>228.363</v>
+      </c>
+      <c r="N18" s="17">
+        <v>258.77300000000002</v>
       </c>
       <c r="O18" s="13" t="s">
-        <v>156</v>
+        <v>59</v>
       </c>
       <c r="P18" s="1">
         <v>0</v>
@@ -1887,19 +1863,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="G19" s="5">
         <v>20101102</v>
@@ -1919,8 +1895,14 @@
       <c r="L19" s="1">
         <v>256</v>
       </c>
+      <c r="M19" s="17">
+        <v>500.56400000000002</v>
+      </c>
+      <c r="N19" s="17">
+        <v>280.85700000000003</v>
+      </c>
       <c r="O19" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P19" s="1">
         <v>1</v>
@@ -1937,19 +1919,19 @@
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="G20" s="5">
         <v>20101102</v>
@@ -1969,8 +1951,14 @@
       <c r="L20" s="1">
         <v>256</v>
       </c>
+      <c r="M20" s="17">
+        <v>478.76900000000001</v>
+      </c>
+      <c r="N20" s="17">
+        <v>357.26400000000001</v>
+      </c>
       <c r="O20" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P20" s="1">
         <v>1</v>
@@ -1987,19 +1975,19 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="G21" s="5">
         <v>20101103</v>
@@ -2019,8 +2007,14 @@
       <c r="L21" s="1">
         <v>256</v>
       </c>
+      <c r="M21" s="17">
+        <v>417.81099999999998</v>
+      </c>
+      <c r="N21" s="17">
+        <v>540.12099999999998</v>
+      </c>
       <c r="O21" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P21" s="1">
         <v>1</v>
@@ -2037,19 +2031,19 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="G22" s="5">
         <v>20101107</v>
@@ -2069,8 +2063,14 @@
       <c r="L22" s="1">
         <v>256</v>
       </c>
+      <c r="M22" s="17">
+        <v>159.11099999999999</v>
+      </c>
+      <c r="N22" s="17">
+        <v>481.61700000000002</v>
+      </c>
       <c r="O22" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P22" s="1">
         <v>1</v>
@@ -2087,40 +2087,46 @@
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>161</v>
+        <v>62</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G23" s="5">
         <v>20110111</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="L23" s="1">
         <v>13</v>
       </c>
+      <c r="M23" s="17">
+        <v>667.13</v>
+      </c>
+      <c r="N23" s="17">
+        <v>662.71199999999999</v>
+      </c>
       <c r="O23" s="13" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
@@ -2137,40 +2143,46 @@
         <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>162</v>
+        <v>63</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G24" s="5">
         <v>20110111</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="L24" s="1">
         <v>13</v>
       </c>
+      <c r="M24" s="17">
+        <v>486.91399999999999</v>
+      </c>
+      <c r="N24" s="17">
+        <v>550.70600000000002</v>
+      </c>
       <c r="O24" s="13" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -2187,19 +2199,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="G25" s="1">
         <v>20110131</v>
@@ -2219,8 +2231,14 @@
       <c r="L25" s="1">
         <v>128</v>
       </c>
+      <c r="M25" s="17">
+        <v>602.04300000000001</v>
+      </c>
+      <c r="N25" s="17">
+        <v>450.29700000000003</v>
+      </c>
       <c r="O25" s="12" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
       <c r="P25" s="1">
         <v>0</v>
@@ -2237,19 +2255,19 @@
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="G26" s="5">
         <v>20110211</v>
@@ -2269,8 +2287,14 @@
       <c r="L26" s="1">
         <v>128</v>
       </c>
+      <c r="M26" s="17">
+        <v>162.297</v>
+      </c>
+      <c r="N26" s="17">
+        <v>519.428</v>
+      </c>
       <c r="O26" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P26" s="1">
         <v>1</v>
@@ -2287,19 +2311,19 @@
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="G27" s="5">
         <v>20110213</v>
@@ -2319,8 +2343,14 @@
       <c r="L27" s="1">
         <v>128</v>
       </c>
+      <c r="M27" s="17">
+        <v>194.34899999999999</v>
+      </c>
+      <c r="N27" s="17">
+        <v>474.51</v>
+      </c>
       <c r="O27" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P27" s="1">
         <v>1</v>
@@ -2337,19 +2367,19 @@
         <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="G28" s="5">
         <v>20110213</v>
@@ -2369,8 +2399,14 @@
       <c r="L28" s="1">
         <v>128</v>
       </c>
+      <c r="M28" s="17">
+        <v>215.87799999999999</v>
+      </c>
+      <c r="N28" s="17">
+        <v>540.74300000000005</v>
+      </c>
       <c r="O28" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P28" s="1">
         <v>1</v>
@@ -2387,19 +2423,19 @@
         <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="G29" s="5">
         <v>20110213</v>
@@ -2419,8 +2455,14 @@
       <c r="L29" s="1">
         <v>128</v>
       </c>
+      <c r="M29" s="17">
+        <v>167.19900000000001</v>
+      </c>
+      <c r="N29" s="17">
+        <v>446.55</v>
+      </c>
       <c r="O29" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P29" s="1">
         <v>1</v>
@@ -2437,19 +2479,19 @@
         <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="G30" s="5">
         <v>20110214</v>
@@ -2469,8 +2511,14 @@
       <c r="L30" s="1">
         <v>128</v>
       </c>
+      <c r="M30" s="17">
+        <v>279.69900000000001</v>
+      </c>
+      <c r="N30" s="17">
+        <v>696.42200000000003</v>
+      </c>
       <c r="O30" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P30" s="1">
         <v>1</v>
@@ -2487,19 +2535,19 @@
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="G31" s="1">
         <v>20110214</v>
@@ -2519,8 +2567,14 @@
       <c r="L31" s="1">
         <v>128</v>
       </c>
+      <c r="M31" s="17">
+        <v>177.59800000000001</v>
+      </c>
+      <c r="N31" s="17">
+        <v>630.096</v>
+      </c>
       <c r="O31" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P31" s="1">
         <v>1</v>
@@ -2537,19 +2591,19 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="G32" s="1">
         <v>20110214</v>
@@ -2569,8 +2623,14 @@
       <c r="L32" s="1">
         <v>128</v>
       </c>
+      <c r="M32" s="17">
+        <v>293.88299999999998</v>
+      </c>
+      <c r="N32" s="17">
+        <v>617.91200000000003</v>
+      </c>
       <c r="O32" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P32" s="1">
         <v>1</v>
@@ -2587,19 +2647,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="G33" s="1">
         <v>20110215</v>
@@ -2619,8 +2679,14 @@
       <c r="L33" s="1">
         <v>128</v>
       </c>
+      <c r="M33" s="17">
+        <v>222.17400000000001</v>
+      </c>
+      <c r="N33" s="17">
+        <v>491.77600000000001</v>
+      </c>
       <c r="O33" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P33" s="1">
         <v>1</v>
@@ -2637,19 +2703,19 @@
         <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>120</v>
+        <v>58</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="G34" s="1">
         <v>20110217</v>
@@ -2669,8 +2735,14 @@
       <c r="L34" s="1">
         <v>128</v>
       </c>
+      <c r="M34" s="17">
+        <v>416.94499999999999</v>
+      </c>
+      <c r="N34" s="17">
+        <v>339.34199999999998</v>
+      </c>
       <c r="O34" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P34" s="1">
         <v>1</v>
@@ -2687,19 +2759,19 @@
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="G35" s="1">
         <v>20110218</v>
@@ -2719,8 +2791,14 @@
       <c r="L35" s="1">
         <v>128</v>
       </c>
+      <c r="M35" s="17">
+        <v>208.708</v>
+      </c>
+      <c r="N35" s="17">
+        <v>758.31799999999998</v>
+      </c>
       <c r="O35" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P35" s="1">
         <v>1</v>
@@ -2737,19 +2815,19 @@
         <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="G36" s="1">
         <v>20110218</v>
@@ -2769,8 +2847,14 @@
       <c r="L36" s="1">
         <v>128</v>
       </c>
+      <c r="M36" s="17">
+        <v>277.43700000000001</v>
+      </c>
+      <c r="N36" s="17">
+        <v>742.60199999999998</v>
+      </c>
       <c r="O36" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P36" s="1">
         <v>1</v>
@@ -2787,19 +2871,19 @@
         <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="G37" s="1">
         <v>20110218</v>
@@ -2819,8 +2903,14 @@
       <c r="L37" s="1">
         <v>128</v>
       </c>
+      <c r="M37" s="17">
+        <v>316.41500000000002</v>
+      </c>
+      <c r="N37" s="17">
+        <v>735.83799999999997</v>
+      </c>
       <c r="O37" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P37" s="1">
         <v>1</v>
@@ -2837,19 +2927,19 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>137</v>
+        <v>70</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="G38" s="1">
         <v>20110218</v>
@@ -2869,8 +2959,14 @@
       <c r="L38" s="1">
         <v>128</v>
       </c>
+      <c r="M38" s="17">
+        <v>184.55099999999999</v>
+      </c>
+      <c r="N38" s="17">
+        <v>738.21199999999999</v>
+      </c>
       <c r="O38" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P38" s="1">
         <v>1</v>
@@ -2887,19 +2983,19 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="G39" s="1">
         <v>20110219</v>
@@ -2919,8 +3015,14 @@
       <c r="L39" s="1">
         <v>128</v>
       </c>
+      <c r="M39" s="17">
+        <v>248.03299999999999</v>
+      </c>
+      <c r="N39" s="17">
+        <v>448.11599999999999</v>
+      </c>
       <c r="O39" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P39" s="1">
         <v>1</v>
@@ -2937,19 +3039,19 @@
         <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="G40" s="1">
         <v>20110219</v>
@@ -2969,8 +3071,14 @@
       <c r="L40" s="1">
         <v>128</v>
       </c>
+      <c r="M40" s="17">
+        <v>142.38900000000001</v>
+      </c>
+      <c r="N40" s="17">
+        <v>170.98699999999999</v>
+      </c>
       <c r="O40" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P40" s="1">
         <v>1</v>
@@ -2987,19 +3095,19 @@
         <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="G41" s="1">
         <v>20110219</v>
@@ -3019,8 +3127,14 @@
       <c r="L41" s="1">
         <v>128</v>
       </c>
+      <c r="M41" s="17">
+        <v>137.80500000000001</v>
+      </c>
+      <c r="N41" s="17">
+        <v>456.57</v>
+      </c>
       <c r="O41" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P41" s="1">
         <v>1</v>
@@ -3037,19 +3151,19 @@
         <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="G42" s="1">
         <v>20110219</v>
@@ -3069,8 +3183,14 @@
       <c r="L42" s="1">
         <v>128</v>
       </c>
+      <c r="M42" s="17">
+        <v>233.17500000000001</v>
+      </c>
+      <c r="N42" s="17">
+        <v>339.42599999999999</v>
+      </c>
       <c r="O42" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P42" s="1">
         <v>1</v>
@@ -3087,19 +3207,19 @@
         <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G43" s="1">
         <v>20110219</v>
@@ -3119,8 +3239,14 @@
       <c r="L43" s="1">
         <v>128</v>
       </c>
+      <c r="M43" s="17">
+        <v>217.34399999999999</v>
+      </c>
+      <c r="N43" s="17">
+        <v>191.54900000000001</v>
+      </c>
       <c r="O43" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P43" s="1">
         <v>1</v>
@@ -3137,19 +3263,19 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G44" s="1">
         <v>20110219</v>
@@ -3169,8 +3295,14 @@
       <c r="L44" s="1">
         <v>128</v>
       </c>
+      <c r="M44" s="17">
+        <v>185.06</v>
+      </c>
+      <c r="N44" s="17">
+        <v>470.45100000000002</v>
+      </c>
       <c r="O44" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P44" s="1">
         <v>1</v>
@@ -3187,19 +3319,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="G45" s="1">
         <v>20110509</v>
@@ -3220,8 +3352,14 @@
       <c r="L45" s="1">
         <v>128</v>
       </c>
+      <c r="M45" s="17">
+        <v>422.95400000000001</v>
+      </c>
+      <c r="N45" s="17">
+        <v>629.98099999999999</v>
+      </c>
       <c r="O45" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P45" s="1">
         <v>1</v>
@@ -3238,19 +3376,19 @@
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="G46" s="5">
         <v>20110510</v>
@@ -3270,8 +3408,14 @@
       <c r="L46" s="1">
         <v>128</v>
       </c>
+      <c r="M46" s="17">
+        <v>428.029</v>
+      </c>
+      <c r="N46" s="17">
+        <v>535.78599999999994</v>
+      </c>
       <c r="O46" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P46" s="1">
         <v>1</v>
@@ -3288,19 +3432,19 @@
         <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="G47" s="1">
         <v>20110510</v>
@@ -3320,8 +3464,14 @@
       <c r="L47" s="1">
         <v>128</v>
       </c>
+      <c r="M47" s="17">
+        <v>354.553</v>
+      </c>
+      <c r="N47" s="17">
+        <v>526.78800000000001</v>
+      </c>
       <c r="O47" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P47" s="1">
         <v>1</v>
@@ -3338,19 +3488,19 @@
         <v>30</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G48" s="1">
         <v>20110511</v>
@@ -3370,8 +3520,14 @@
       <c r="L48" s="1">
         <v>128</v>
       </c>
+      <c r="M48" s="17">
+        <v>340.94400000000002</v>
+      </c>
+      <c r="N48" s="17">
+        <v>516.221</v>
+      </c>
       <c r="O48" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P48" s="1">
         <v>1</v>
@@ -3388,19 +3544,19 @@
         <v>34</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G49" s="1">
         <v>20110511</v>
@@ -3420,8 +3576,14 @@
       <c r="L49" s="1">
         <v>128</v>
       </c>
+      <c r="M49" s="17">
+        <v>359.33100000000002</v>
+      </c>
+      <c r="N49" s="17">
+        <v>550.49800000000005</v>
+      </c>
       <c r="O49" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P49" s="1">
         <v>1</v>
@@ -3438,19 +3600,19 @@
         <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G50" s="1">
         <v>20110512</v>
@@ -3470,8 +3632,14 @@
       <c r="L50" s="1">
         <v>128</v>
       </c>
+      <c r="M50" s="17">
+        <v>284.46600000000001</v>
+      </c>
+      <c r="N50" s="17">
+        <v>536.69000000000005</v>
+      </c>
       <c r="O50" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P50" s="1">
         <v>1</v>
@@ -3488,19 +3656,19 @@
         <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="G51" s="1">
         <v>20110513</v>
@@ -3520,8 +3688,14 @@
       <c r="L51" s="1">
         <v>128</v>
       </c>
+      <c r="M51" s="17">
+        <v>173.976</v>
+      </c>
+      <c r="N51" s="17">
+        <v>611.78700000000003</v>
+      </c>
       <c r="O51" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P51" s="1">
         <v>1</v>
@@ -3538,19 +3712,19 @@
         <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G52" s="1">
         <v>20110513</v>
@@ -3570,8 +3744,14 @@
       <c r="L52" s="1">
         <v>128</v>
       </c>
+      <c r="M52" s="17">
+        <v>248.703</v>
+      </c>
+      <c r="N52" s="17">
+        <v>763.05399999999997</v>
+      </c>
       <c r="O52" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P52" s="1">
         <v>1</v>
@@ -3588,19 +3768,19 @@
         <v>35</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="G53" s="1">
         <v>20110513</v>
@@ -3620,8 +3800,14 @@
       <c r="L53" s="1">
         <v>5</v>
       </c>
+      <c r="M53" s="17">
+        <v>301.39999999999998</v>
+      </c>
+      <c r="N53" s="17">
+        <v>598.1</v>
+      </c>
       <c r="O53" s="13" t="s">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="P53" s="1">
         <v>0</v>
@@ -3638,19 +3824,19 @@
         <v>37</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="G54" s="5">
         <v>20110513</v>
@@ -3670,8 +3856,14 @@
       <c r="L54" s="1">
         <v>3</v>
       </c>
+      <c r="M54" s="17">
+        <v>109.2</v>
+      </c>
+      <c r="N54" s="17">
+        <v>584.1</v>
+      </c>
       <c r="O54" s="13" t="s">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="P54" s="1">
         <v>0</v>
@@ -3688,19 +3880,19 @@
         <v>43</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="G55" s="5">
         <v>20110613</v>
@@ -3721,8 +3913,14 @@
       <c r="L55" s="1">
         <v>128</v>
       </c>
+      <c r="M55" s="17">
+        <v>418.036</v>
+      </c>
+      <c r="N55" s="17">
+        <v>602.95399999999995</v>
+      </c>
       <c r="O55" s="12" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
       <c r="P55" s="1">
         <v>0</v>
@@ -3739,19 +3937,19 @@
         <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="G56" s="5">
         <v>20110930</v>
@@ -3772,8 +3970,14 @@
       <c r="L56" s="1">
         <v>256</v>
       </c>
+      <c r="M56" s="17">
+        <v>280.04599999999999</v>
+      </c>
+      <c r="N56" s="17">
+        <v>659.58500000000004</v>
+      </c>
       <c r="O56" s="12" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="P56" s="1">
         <v>0</v>
@@ -3790,19 +3994,19 @@
         <v>50</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>207</v>
+        <v>79</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G57" s="1">
         <v>20130423</v>
@@ -3822,8 +4026,14 @@
       <c r="L57" s="1">
         <v>256</v>
       </c>
+      <c r="M57" s="17">
+        <v>421.16699999999997</v>
+      </c>
+      <c r="N57" s="17">
+        <v>480</v>
+      </c>
       <c r="O57" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P57" s="1">
         <v>0</v>
@@ -3840,19 +4050,19 @@
         <v>47</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="G58" s="1">
         <v>20130627</v>
@@ -3873,8 +4083,14 @@
       <c r="L58" s="1">
         <v>256</v>
       </c>
+      <c r="M58" s="17">
+        <v>564.68100000000004</v>
+      </c>
+      <c r="N58" s="17">
+        <v>555.56799999999998</v>
+      </c>
       <c r="O58" s="12" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
       <c r="P58" s="1">
         <v>0</v>
@@ -3891,19 +4107,19 @@
         <v>48</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>201</v>
+        <v>81</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="G59" s="1">
         <v>20130627</v>
@@ -3924,8 +4140,14 @@
       <c r="L59" s="1">
         <v>256</v>
       </c>
+      <c r="M59" s="17">
+        <v>541.12599999999998</v>
+      </c>
+      <c r="N59" s="17">
+        <v>492.767</v>
+      </c>
       <c r="O59" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P59" s="1">
         <v>0</v>
@@ -3942,19 +4164,19 @@
         <v>49</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="G60" s="1">
         <v>20130628</v>
@@ -3974,14 +4196,20 @@
       <c r="L60" s="1">
         <v>256</v>
       </c>
+      <c r="M60" s="17">
+        <v>571.20000000000005</v>
+      </c>
+      <c r="N60" s="17">
+        <v>540.20000000000005</v>
+      </c>
       <c r="O60" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P60" s="1">
         <v>0</v>
       </c>
       <c r="Q60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R60" s="1">
         <v>1</v>
@@ -3992,19 +4220,19 @@
         <v>51</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>207</v>
+        <v>0</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G61" s="1">
         <v>20130703</v>
@@ -4024,8 +4252,14 @@
       <c r="L61" s="1">
         <v>256</v>
       </c>
+      <c r="M61" s="17">
+        <v>617.10199999999998</v>
+      </c>
+      <c r="N61" s="17">
+        <v>614.49199999999996</v>
+      </c>
       <c r="O61" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P61" s="1">
         <v>0</v>
@@ -4042,19 +4276,19 @@
         <v>52</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="G62" s="1">
         <v>20130705</v>
@@ -4074,8 +4308,14 @@
       <c r="L62" s="1">
         <v>256</v>
       </c>
+      <c r="M62" s="17">
+        <v>497.40300000000002</v>
+      </c>
+      <c r="N62" s="17">
+        <v>578.38499999999999</v>
+      </c>
       <c r="O62" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P62" s="1">
         <v>0</v>
@@ -4092,19 +4332,19 @@
         <v>53</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="G63" s="1">
         <v>20130827</v>
@@ -4124,8 +4364,14 @@
       <c r="L63" s="1">
         <v>256</v>
       </c>
+      <c r="M63" s="17">
+        <v>506.89699999999999</v>
+      </c>
+      <c r="N63" s="17">
+        <v>525.91099999999994</v>
+      </c>
       <c r="O63" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P63" s="1">
         <v>0</v>
@@ -4142,19 +4388,19 @@
         <v>55</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>222</v>
+        <v>35</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>221</v>
+        <v>1</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>222</v>
+        <v>35</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>219</v>
+        <v>2</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="G64" s="1">
         <v>20130830</v>
@@ -4169,19 +4415,25 @@
         <v>838</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>223</v>
+        <v>3</v>
       </c>
       <c r="L64" s="1">
         <v>999</v>
       </c>
+      <c r="M64" s="17">
+        <v>1014.07</v>
+      </c>
+      <c r="N64" s="17">
+        <v>291.84899999999999</v>
+      </c>
       <c r="O64" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P64" s="1">
         <v>0</v>
       </c>
       <c r="Q64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R64" s="1">
         <v>0</v>
@@ -4192,19 +4444,19 @@
         <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>224</v>
+        <v>19</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>189</v>
+        <v>58</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>140</v>
+        <v>25</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G65" s="1">
         <v>20131014</v>
@@ -4224,8 +4476,14 @@
       <c r="L65" s="1">
         <v>256</v>
       </c>
+      <c r="M65" s="17">
+        <v>488.3</v>
+      </c>
+      <c r="N65" s="17">
+        <v>612.20000000000005</v>
+      </c>
       <c r="O65" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P65" s="1">
         <v>0</v>
@@ -4242,19 +4500,19 @@
         <v>58</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="G66" s="1">
         <v>20131016</v>
@@ -4275,8 +4533,14 @@
       <c r="L66" s="1">
         <v>256</v>
       </c>
+      <c r="M66" s="17">
+        <v>418.58300000000003</v>
+      </c>
+      <c r="N66" s="17">
+        <v>372.16199999999998</v>
+      </c>
       <c r="O66" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P66" s="1">
         <v>0</v>
@@ -4293,19 +4557,19 @@
         <v>57</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="G67" s="1">
         <v>20131108</v>
@@ -4326,8 +4590,14 @@
       <c r="L67" s="1">
         <v>256</v>
       </c>
+      <c r="M67" s="17">
+        <v>693.86199999999997</v>
+      </c>
+      <c r="N67" s="17">
+        <v>502.38200000000001</v>
+      </c>
       <c r="O67" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P67" s="1">
         <v>0</v>
@@ -4344,19 +4614,19 @@
         <v>60</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>197</v>
+        <v>24</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G68" s="1">
         <v>20131202</v>
@@ -4376,8 +4646,14 @@
       <c r="L68" s="1">
         <v>256</v>
       </c>
+      <c r="M68" s="17">
+        <v>540.50199999999995</v>
+      </c>
+      <c r="N68" s="17">
+        <v>461.04</v>
+      </c>
       <c r="O68" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P68" s="1">
         <v>0</v>
@@ -4394,19 +4670,19 @@
         <v>59</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>207</v>
+        <v>79</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>194</v>
+        <v>21</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G69" s="1">
         <v>20131203</v>
@@ -4426,8 +4702,14 @@
       <c r="L69" s="1">
         <v>256</v>
       </c>
+      <c r="M69" s="17">
+        <v>572.78200000000004</v>
+      </c>
+      <c r="N69" s="17">
+        <v>566.50300000000004</v>
+      </c>
       <c r="O69" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P69" s="1">
         <v>0</v>
@@ -4444,19 +4726,19 @@
         <v>61</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>207</v>
+        <v>79</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G70" s="1">
         <v>20140113</v>
@@ -4476,8 +4758,14 @@
       <c r="L70" s="1">
         <v>256</v>
       </c>
+      <c r="M70" s="17">
+        <v>288.02600000000001</v>
+      </c>
+      <c r="N70" s="17">
+        <v>477.20699999999999</v>
+      </c>
       <c r="O70" s="12" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="P70" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
add  f_reduce flag and associated code, and some minor cleanup of code
</commit_message>
<xml_diff>
--- a/mSPAGHETI_analysis_log_2014b.xlsx
+++ b/mSPAGHETI_analysis_log_2014b.xlsx
@@ -19,7 +19,417 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="208">
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130827_mir/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/sim_grate/A6I_scattered/scattered/</t>
+  </si>
+  <si>
+    <t>scattered-</t>
+  </si>
+  <si>
+    <t>mask200um_top10um_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131203/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20140113/SIGRTUTIShell_JHK_B/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All data present</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/G02_optical/</t>
+  </si>
+  <si>
+    <t>G02_R3_d15mm_w632nm_f838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G03/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_E_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_F/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_F_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A/</t>
+  </si>
+  <si>
+    <t>TJ07_A_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A_f200mm/</t>
+  </si>
+  <si>
+    <t>TJ07_A_d6mm_f200mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B/</t>
+  </si>
+  <si>
+    <t>TJ07_B_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B_f200mm/</t>
+  </si>
+  <si>
+    <t>TJ07_B_d6mm_f200mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C/</t>
+  </si>
+  <si>
+    <t>TJ07_C_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C_f200mm/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131016/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20131108/</t>
+  </si>
+  <si>
+    <t>mirror_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>JHKishell_d5mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>Mirror_d5mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>JHKishell_d5mm_L632_f838_B-</t>
+  </si>
+  <si>
+    <t>G03_R3_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G05/</t>
+  </si>
+  <si>
+    <t>G05_R3_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130628_mir/</t>
+  </si>
+  <si>
+    <t>mir_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130423_ishell_JHK/</t>
+  </si>
+  <si>
+    <t>ishell_JHK_JPL_wafer_R1p4_d6mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130703/</t>
+  </si>
+  <si>
+    <t>ishellJHK_d6mm_L632_f838_R1p4-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130705_mir/</t>
+  </si>
+  <si>
+    <t>mir_d6mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D_f200mm/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100217/</t>
+  </si>
+  <si>
+    <t>G1_L632nm_f400mm_d15mm_R2-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100220/</t>
+  </si>
+  <si>
+    <t>G1_L543nm_f400mm_d15mm_R2-</t>
+  </si>
+  <si>
+    <t>E06_632nm_25mm_2000mm_hdr-</t>
+  </si>
+  <si>
+    <t>TJ03F_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_G/</t>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ03G_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_H/</t>
+  </si>
+  <si>
+    <t>TJ03H_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110215/</t>
+  </si>
+  <si>
+    <t>TJ03E_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110217_mir/</t>
+  </si>
+  <si>
+    <t>mirror_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_G/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_G_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_H/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_H_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_I/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_I_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>TJ04_25um_J_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_A/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_A_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_B/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_B_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_C/</t>
+  </si>
+  <si>
+    <t>E09_R3_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>E12_R3_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100626/</t>
+  </si>
+  <si>
+    <t>E06_632nm_20mm_838mm_hdr-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E10/E10/</t>
+  </si>
+  <si>
+    <t>E10_20mm_632nm_838mm_R3-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E11/20110613/</t>
+  </si>
+  <si>
+    <t>E11_R3_d25mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/20110111/</t>
+  </si>
+  <si>
+    <t>g02_angle_pos1_dither1-</t>
+  </si>
+  <si>
+    <t>g02_angle_pos2_dither1-</t>
+  </si>
+  <si>
+    <t>All data present, "G" instead of "D" as suffix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JHK_JPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/MIT/UTN18/20110131/</t>
+  </si>
+  <si>
+    <t>utn18_f838_L632_d15mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110509/</t>
+  </si>
+  <si>
+    <t>E09_R3_d25mm_f838mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110510/</t>
+  </si>
+  <si>
+    <t>E09_m0_d20mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dithered, see notes in .ppt document</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Author:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gully</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Date:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ04_100um_C_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_D/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_D_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_E/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20110930/</t>
+  </si>
+  <si>
+    <t>E12_D25mm_f2m_l632nm_R3-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101028/</t>
+  </si>
+  <si>
+    <t>JPL01_A100um_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>mir_D12_5mm_L632nm_F838mm_dith-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101102/</t>
+  </si>
+  <si>
+    <t>TJ01B_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/mir/</t>
+  </si>
+  <si>
+    <t>mir_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101103/</t>
+  </si>
+  <si>
+    <t>TJ02B_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101107/</t>
+  </si>
+  <si>
+    <t>TJ02A_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110211/</t>
+  </si>
+  <si>
+    <t>TJ03_blaze_d8_2mm_l632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213/</t>
+  </si>
+  <si>
+    <t>TJ03A_blaze_d8_2mm_l632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_C/</t>
+  </si>
+  <si>
+    <t>TJ03C_blaze_d8_2mm_l632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_D/</t>
+  </si>
+  <si>
+    <t>TJ03D_blaze_d8_2mm_l632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_F/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D/</t>
+  </si>
+  <si>
+    <t>TJ07_d6mm_f838mm_632nm-</t>
+  </si>
   <si>
     <t>JHK_JPL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -342,406 +752,6 @@
     <t>E12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>All data present, "G" instead of "D" as suffix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JHK_JPL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/MIT/UTN18/20110131/</t>
-  </si>
-  <si>
-    <t>utn18_f838_L632_d15mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110509/</t>
-  </si>
-  <si>
-    <t>E09_R3_d25mm_f838mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110510/</t>
-  </si>
-  <si>
-    <t>E09_m0_d20mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dithered, see notes in .ppt document</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Author:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gully</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Date:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ04_100um_C_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_D/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_D_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_E/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20110930/</t>
-  </si>
-  <si>
-    <t>E12_D25mm_f2m_l632nm_R3-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101028/</t>
-  </si>
-  <si>
-    <t>JPL01_A100um_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>mir_D12_5mm_L632nm_F838mm_dith-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101102/</t>
-  </si>
-  <si>
-    <t>TJ01B_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/mir/</t>
-  </si>
-  <si>
-    <t>mir_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101103/</t>
-  </si>
-  <si>
-    <t>TJ02B_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101107/</t>
-  </si>
-  <si>
-    <t>TJ02A_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110211/</t>
-  </si>
-  <si>
-    <t>TJ03_blaze_d8_2mm_l632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213/</t>
-  </si>
-  <si>
-    <t>TJ03A_blaze_d8_2mm_l632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_C/</t>
-  </si>
-  <si>
-    <t>TJ03C_blaze_d8_2mm_l632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_D/</t>
-  </si>
-  <si>
-    <t>TJ03D_blaze_d8_2mm_l632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_F/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D/</t>
-  </si>
-  <si>
-    <t>TJ07_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D_f200mm/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100217/</t>
-  </si>
-  <si>
-    <t>G1_L632nm_f400mm_d15mm_R2-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100220/</t>
-  </si>
-  <si>
-    <t>G1_L543nm_f400mm_d15mm_R2-</t>
-  </si>
-  <si>
-    <t>E06_632nm_25mm_2000mm_hdr-</t>
-  </si>
-  <si>
-    <t>TJ03F_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_G/</t>
-  </si>
-  <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ03G_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_H/</t>
-  </si>
-  <si>
-    <t>TJ03H_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110215/</t>
-  </si>
-  <si>
-    <t>TJ03E_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110217_mir/</t>
-  </si>
-  <si>
-    <t>mirror_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_G/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_G_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_H/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_H_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_I/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_I_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>TJ04_25um_J_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_A/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_A_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_B/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_B_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_C/</t>
-  </si>
-  <si>
-    <t>E09_R3_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>E12_R3_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100626/</t>
-  </si>
-  <si>
-    <t>E06_632nm_20mm_838mm_hdr-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E10/E10/</t>
-  </si>
-  <si>
-    <t>E10_20mm_632nm_838mm_R3-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E11/20110613/</t>
-  </si>
-  <si>
-    <t>E11_R3_d25mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/20110111/</t>
-  </si>
-  <si>
-    <t>g02_angle_pos1_dither1-</t>
-  </si>
-  <si>
-    <t>g02_angle_pos2_dither1-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/G02_optical/</t>
-  </si>
-  <si>
-    <t>G02_R3_d15mm_w632nm_f838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G03/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_E_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_F/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_F_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A/</t>
-  </si>
-  <si>
-    <t>TJ07_A_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A_f200mm/</t>
-  </si>
-  <si>
-    <t>TJ07_A_d6mm_f200mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B/</t>
-  </si>
-  <si>
-    <t>TJ07_B_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B_f200mm/</t>
-  </si>
-  <si>
-    <t>TJ07_B_d6mm_f200mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C/</t>
-  </si>
-  <si>
-    <t>TJ07_C_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C_f200mm/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131016/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20131108/</t>
-  </si>
-  <si>
-    <t>mirror_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>JHKishell_d5mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>Mirror_d5mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>JHKishell_d5mm_L632_f838_B-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131203</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20140113/SIGRTUTIShell_JHK_B</t>
-  </si>
-  <si>
-    <t>G03_R3_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G05/</t>
-  </si>
-  <si>
-    <t>G05_R3_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130628_mir/</t>
-  </si>
-  <si>
-    <t>mir_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130423_ishell_JHK/</t>
-  </si>
-  <si>
-    <t>ishell_JHK_JPL_wafer_R1p4_d6mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130703/</t>
-  </si>
-  <si>
-    <t>ishellJHK_d6mm_L632_f838_R1p4-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130705_mir/</t>
-  </si>
-  <si>
-    <t>mir_d6mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130827_mir/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/sim_grate/A6I_scattered/scattered/</t>
-  </si>
-  <si>
-    <t>scattered-</t>
-  </si>
-  <si>
-    <t>mask200um_top10um_d25mm_L632_f838-</t>
-  </si>
 </sst>
 </file>
 
@@ -752,8 +762,8 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -814,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -830,7 +840,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -840,7 +850,8 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:R107"/>
+  <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="O3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1181,191 +1192,194 @@
     <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" style="1"/>
     <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="40.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1"/>
     <col min="8" max="8" width="6" style="1" customWidth="1"/>
     <col min="9" max="10" width="5.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="4.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.28515625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="6.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="9.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="5.42578125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.7109375" style="1"/>
+    <col min="19" max="19" width="6.5703125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2">
         <v>40190</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>156</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="Q6" s="8"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7" s="14" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="S7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>147</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>38</v>
+        <v>168</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>41</v>
+        <v>171</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1">
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="G10" s="5">
         <v>20100217</v>
@@ -1379,7 +1393,7 @@
       <c r="J10" s="1">
         <v>400</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="18">
         <f>ATAN(2)*180/PI()</f>
         <v>63.43494882292201</v>
       </c>
@@ -1393,7 +1407,7 @@
         <v>445.50299999999999</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P10" s="1">
         <v>1</v>
@@ -1404,25 +1418,28 @@
       <c r="R10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1">
         <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>174</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="G11" s="5">
         <v>20100220</v>
@@ -1436,7 +1453,7 @@
       <c r="J11" s="1">
         <v>400</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="18">
         <f>ATAN(2)*180/PI()</f>
         <v>63.43494882292201</v>
       </c>
@@ -1450,7 +1467,7 @@
         <v>485.83199999999999</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P11" s="1">
         <v>1</v>
@@ -1461,25 +1478,28 @@
       <c r="R11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1">
         <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="G12" s="5">
         <v>20100624</v>
@@ -1493,7 +1513,7 @@
       <c r="J12" s="1">
         <v>2000</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -1507,7 +1527,7 @@
         <v>431.52600000000001</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P12" s="1">
         <v>1</v>
@@ -1518,25 +1538,28 @@
       <c r="R12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="1">
         <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>157</v>
+        <v>77</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>158</v>
+        <v>78</v>
       </c>
       <c r="G13" s="5">
         <v>20100626</v>
@@ -1550,7 +1573,7 @@
       <c r="J13" s="1">
         <v>828</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -1564,7 +1587,7 @@
         <v>291.541</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P13" s="1">
         <v>1</v>
@@ -1575,25 +1598,28 @@
       <c r="R13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1">
         <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>167</v>
+        <v>9</v>
       </c>
       <c r="G14" s="1">
         <v>20100719</v>
@@ -1607,7 +1633,7 @@
       <c r="J14" s="1">
         <v>838</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -1621,7 +1647,7 @@
         <v>426.42599999999999</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P14" s="1">
         <v>1</v>
@@ -1632,40 +1658,43 @@
       <c r="R14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="1">
         <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>203</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>204</v>
+        <v>2</v>
       </c>
       <c r="G15" s="1">
         <v>20100817</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>51</v>
+        <v>181</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>52</v>
+        <v>182</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>19</v>
+        <v>148</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="L15" s="1">
         <v>500</v>
@@ -1677,7 +1706,7 @@
         <v>707.85699999999997</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>53</v>
+        <v>183</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
@@ -1688,25 +1717,28 @@
       <c r="R15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1">
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>159</v>
+        <v>79</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="G16" s="5">
         <v>20100824</v>
@@ -1720,7 +1752,7 @@
       <c r="J16" s="1">
         <v>838</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -1734,7 +1766,7 @@
         <v>390.601</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P16" s="1">
         <v>1</v>
@@ -1745,25 +1777,28 @@
       <c r="R16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>186</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>187</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G17" s="5">
         <v>20101028</v>
@@ -1777,7 +1812,7 @@
       <c r="J17" s="10">
         <v>838</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="18">
         <v>54.7</v>
       </c>
       <c r="L17" s="1">
@@ -1790,7 +1825,7 @@
         <v>691.86699999999996</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P17" s="1">
         <v>1</v>
@@ -1801,25 +1836,28 @@
       <c r="R17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="1">
         <v>6</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="G18" s="5">
         <v>20101028</v>
@@ -1833,7 +1871,7 @@
       <c r="J18" s="10">
         <v>838</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="18">
         <v>0</v>
       </c>
       <c r="L18" s="1">
@@ -1846,7 +1884,7 @@
         <v>258.77300000000002</v>
       </c>
       <c r="O18" s="13" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="P18" s="1">
         <v>0</v>
@@ -1857,25 +1895,28 @@
       <c r="R18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="1">
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="G19" s="5">
         <v>20101102</v>
@@ -1889,7 +1930,7 @@
       <c r="J19" s="10">
         <v>838</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="18">
         <v>54.7</v>
       </c>
       <c r="L19" s="1">
@@ -1902,7 +1943,7 @@
         <v>280.85700000000003</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P19" s="1">
         <v>1</v>
@@ -1913,25 +1954,28 @@
       <c r="R19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="1">
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G20" s="5">
         <v>20101102</v>
@@ -1945,7 +1989,7 @@
       <c r="J20" s="10">
         <v>838</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="18">
         <v>0</v>
       </c>
       <c r="L20" s="1">
@@ -1958,7 +2002,7 @@
         <v>357.26400000000001</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P20" s="1">
         <v>1</v>
@@ -1969,25 +2013,28 @@
       <c r="R20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="1">
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>191</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G21" s="5">
         <v>20101103</v>
@@ -2001,7 +2048,7 @@
       <c r="J21" s="10">
         <v>838</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="18">
         <v>54.7</v>
       </c>
       <c r="L21" s="1">
@@ -2014,7 +2061,7 @@
         <v>540.12099999999998</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P21" s="1">
         <v>1</v>
@@ -2025,25 +2072,28 @@
       <c r="R21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="1">
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>191</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G22" s="5">
         <v>20101107</v>
@@ -2057,7 +2107,7 @@
       <c r="J22" s="10">
         <v>838</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="18">
         <v>54.7</v>
       </c>
       <c r="L22" s="1">
@@ -2069,8 +2119,8 @@
       <c r="N22" s="17">
         <v>481.61700000000002</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>43</v>
+      <c r="O22" s="1">
+        <v>2014</v>
       </c>
       <c r="P22" s="1">
         <v>1</v>
@@ -2081,40 +2131,43 @@
       <c r="R22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="S22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="1">
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>62</v>
+        <v>192</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>164</v>
+        <v>84</v>
       </c>
       <c r="G23" s="5">
         <v>20110111</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>19</v>
+        <v>149</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="L23" s="1">
         <v>13</v>
@@ -2126,7 +2179,7 @@
         <v>662.71199999999999</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
@@ -2137,40 +2190,43 @@
       <c r="R23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="1">
         <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>63</v>
+        <v>193</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>165</v>
+        <v>85</v>
       </c>
       <c r="G24" s="5">
         <v>20110111</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>19</v>
+        <v>149</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="L24" s="1">
         <v>13</v>
@@ -2182,7 +2238,7 @@
         <v>550.70600000000002</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -2193,25 +2249,28 @@
       <c r="R24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="1">
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>194</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="G25" s="1">
         <v>20110131</v>
@@ -2225,7 +2284,7 @@
       <c r="J25" s="10">
         <v>838</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="18">
         <v>54.7</v>
       </c>
       <c r="L25" s="1">
@@ -2238,7 +2297,7 @@
         <v>450.29700000000003</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P25" s="1">
         <v>0</v>
@@ -2249,25 +2308,28 @@
       <c r="R25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="S25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="1">
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="G26" s="5">
         <v>20110211</v>
@@ -2281,7 +2343,7 @@
       <c r="J26" s="10">
         <v>200</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="18">
         <v>54.7</v>
       </c>
       <c r="L26" s="1">
@@ -2294,7 +2356,7 @@
         <v>519.428</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P26" s="1">
         <v>1</v>
@@ -2305,25 +2367,28 @@
       <c r="R26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="S26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="1">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="G27" s="5">
         <v>20110213</v>
@@ -2337,7 +2402,7 @@
       <c r="J27" s="10">
         <v>200</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="18">
         <v>54.7</v>
       </c>
       <c r="L27" s="1">
@@ -2350,7 +2415,7 @@
         <v>474.51</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P27" s="1">
         <v>1</v>
@@ -2361,25 +2426,28 @@
       <c r="R27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="S27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="1">
         <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>22</v>
+        <v>152</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="G28" s="5">
         <v>20110213</v>
@@ -2393,7 +2461,7 @@
       <c r="J28" s="10">
         <v>200</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="18">
         <v>54.7</v>
       </c>
       <c r="L28" s="1">
@@ -2406,7 +2474,7 @@
         <v>540.74300000000005</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P28" s="1">
         <v>1</v>
@@ -2417,25 +2485,28 @@
       <c r="R28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18">
+      <c r="S28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="1">
         <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>23</v>
+        <v>153</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G29" s="5">
         <v>20110213</v>
@@ -2449,7 +2520,7 @@
       <c r="J29" s="10">
         <v>200</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="18">
         <v>54.7</v>
       </c>
       <c r="L29" s="1">
@@ -2462,7 +2533,7 @@
         <v>446.55</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P29" s="1">
         <v>1</v>
@@ -2473,25 +2544,28 @@
       <c r="R29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="1">
         <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>129</v>
+        <v>49</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="G30" s="5">
         <v>20110214</v>
@@ -2505,7 +2579,7 @@
       <c r="J30" s="10">
         <v>200</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="18">
         <v>54.7</v>
       </c>
       <c r="L30" s="1">
@@ -2518,7 +2592,7 @@
         <v>696.42200000000003</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P30" s="1">
         <v>1</v>
@@ -2529,25 +2603,28 @@
       <c r="R30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="S30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="1">
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>131</v>
+        <v>51</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>134</v>
+        <v>54</v>
       </c>
       <c r="G31" s="1">
         <v>20110214</v>
@@ -2561,7 +2638,7 @@
       <c r="J31" s="10">
         <v>200</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="18">
         <v>54.7</v>
       </c>
       <c r="L31" s="1">
@@ -2574,7 +2651,7 @@
         <v>630.096</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P31" s="1">
         <v>1</v>
@@ -2585,25 +2662,28 @@
       <c r="R31" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="S31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="1">
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>135</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>136</v>
+        <v>56</v>
       </c>
       <c r="G32" s="1">
         <v>20110214</v>
@@ -2617,7 +2697,7 @@
       <c r="J32" s="10">
         <v>200</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="18">
         <v>54.7</v>
       </c>
       <c r="L32" s="1">
@@ -2630,7 +2710,7 @@
         <v>617.91200000000003</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P32" s="1">
         <v>1</v>
@@ -2641,25 +2721,28 @@
       <c r="R32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:18">
+      <c r="S32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="1">
         <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>138</v>
+        <v>58</v>
       </c>
       <c r="G33" s="1">
         <v>20110215</v>
@@ -2673,7 +2756,7 @@
       <c r="J33" s="10">
         <v>200</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="18">
         <v>54.7</v>
       </c>
       <c r="L33" s="1">
@@ -2686,7 +2769,7 @@
         <v>491.77600000000001</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P33" s="1">
         <v>1</v>
@@ -2697,25 +2780,28 @@
       <c r="R33" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:18">
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="1">
         <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>139</v>
+        <v>59</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="G34" s="1">
         <v>20110217</v>
@@ -2729,7 +2815,7 @@
       <c r="J34" s="10">
         <v>200</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="18">
         <v>54.7</v>
       </c>
       <c r="L34" s="1">
@@ -2742,7 +2828,7 @@
         <v>339.34199999999998</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P34" s="1">
         <v>1</v>
@@ -2753,25 +2839,28 @@
       <c r="R34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:18">
+      <c r="S34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="1">
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>131</v>
+        <v>51</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="G35" s="1">
         <v>20110218</v>
@@ -2785,7 +2874,7 @@
       <c r="J35" s="10">
         <v>200</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="18">
         <v>54.7</v>
       </c>
       <c r="L35" s="1">
@@ -2798,7 +2887,7 @@
         <v>758.31799999999998</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P35" s="1">
         <v>1</v>
@@ -2809,25 +2898,28 @@
       <c r="R35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:18">
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="1">
         <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>143</v>
+        <v>63</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>144</v>
+        <v>64</v>
       </c>
       <c r="G36" s="1">
         <v>20110218</v>
@@ -2841,7 +2933,7 @@
       <c r="J36" s="10">
         <v>200</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="18">
         <v>54.7</v>
       </c>
       <c r="L36" s="1">
@@ -2854,7 +2946,7 @@
         <v>742.60199999999998</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P36" s="1">
         <v>1</v>
@@ -2865,25 +2957,28 @@
       <c r="R36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:18">
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="1">
         <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>145</v>
+        <v>65</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="G37" s="1">
         <v>20110218</v>
@@ -2897,7 +2992,7 @@
       <c r="J37" s="10">
         <v>200</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="18">
         <v>54.7</v>
       </c>
       <c r="L37" s="1">
@@ -2910,7 +3005,7 @@
         <v>735.83799999999997</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P37" s="1">
         <v>1</v>
@@ -2921,25 +3016,28 @@
       <c r="R37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:18">
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="1">
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G38" s="1">
         <v>20110218</v>
@@ -2953,7 +3051,7 @@
       <c r="J38" s="10">
         <v>200</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="18">
         <v>54.7</v>
       </c>
       <c r="L38" s="1">
@@ -2966,7 +3064,7 @@
         <v>738.21199999999999</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P38" s="1">
         <v>1</v>
@@ -2977,25 +3075,28 @@
       <c r="R38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:18">
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="1">
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>151</v>
+        <v>71</v>
       </c>
       <c r="G39" s="1">
         <v>20110219</v>
@@ -3009,7 +3110,7 @@
       <c r="J39" s="10">
         <v>838</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39" s="18">
         <v>54.7</v>
       </c>
       <c r="L39" s="1">
@@ -3022,7 +3123,7 @@
         <v>448.11599999999999</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P39" s="1">
         <v>1</v>
@@ -3033,25 +3134,28 @@
       <c r="R39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:18">
+      <c r="S39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="1">
         <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>152</v>
+        <v>72</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="G40" s="1">
         <v>20110219</v>
@@ -3065,7 +3169,7 @@
       <c r="J40" s="10">
         <v>838</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="18">
         <v>54.7</v>
       </c>
       <c r="L40" s="1">
@@ -3078,7 +3182,7 @@
         <v>170.98699999999999</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P40" s="1">
         <v>1</v>
@@ -3089,25 +3193,28 @@
       <c r="R40" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:18">
+      <c r="S40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="1">
         <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>22</v>
+        <v>152</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>154</v>
+        <v>74</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G41" s="1">
         <v>20110219</v>
@@ -3121,7 +3228,7 @@
       <c r="J41" s="10">
         <v>838</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="18">
         <v>54.7</v>
       </c>
       <c r="L41" s="1">
@@ -3134,7 +3241,7 @@
         <v>456.57</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P41" s="1">
         <v>1</v>
@@ -3145,25 +3252,28 @@
       <c r="R41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:18">
+      <c r="S41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="1">
         <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>23</v>
+        <v>153</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G42" s="1">
         <v>20110219</v>
@@ -3177,7 +3287,7 @@
       <c r="J42" s="10">
         <v>838</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="18">
         <v>54.7</v>
       </c>
       <c r="L42" s="1">
@@ -3190,7 +3300,7 @@
         <v>339.42599999999999</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P42" s="1">
         <v>1</v>
@@ -3201,25 +3311,28 @@
       <c r="R42" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:18">
+      <c r="S42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="1">
         <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="G43" s="1">
         <v>20110219</v>
@@ -3233,7 +3346,7 @@
       <c r="J43" s="10">
         <v>838</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="18">
         <v>54.7</v>
       </c>
       <c r="L43" s="1">
@@ -3246,7 +3359,7 @@
         <v>191.54900000000001</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P43" s="1">
         <v>1</v>
@@ -3257,25 +3370,28 @@
       <c r="R43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:18">
+      <c r="S43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="1">
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>129</v>
+        <v>49</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="G44" s="1">
         <v>20110219</v>
@@ -3289,7 +3405,7 @@
       <c r="J44" s="10">
         <v>838</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="18">
         <v>54.7</v>
       </c>
       <c r="L44" s="1">
@@ -3302,7 +3418,7 @@
         <v>470.45100000000002</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P44" s="1">
         <v>1</v>
@@ -3313,25 +3429,28 @@
       <c r="R44" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:18">
+      <c r="S44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="1">
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>71</v>
+        <v>201</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="G45" s="1">
         <v>20110509</v>
@@ -3345,7 +3464,7 @@
       <c r="J45" s="10">
         <v>838</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -3359,7 +3478,7 @@
         <v>629.98099999999999</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P45" s="1">
         <v>1</v>
@@ -3370,25 +3489,28 @@
       <c r="R45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:18">
+      <c r="S45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" s="1">
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>71</v>
+        <v>201</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="G46" s="5">
         <v>20110510</v>
@@ -3402,7 +3524,7 @@
       <c r="J46" s="10">
         <v>838</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="18">
         <v>0</v>
       </c>
       <c r="L46" s="1">
@@ -3415,7 +3537,7 @@
         <v>535.78599999999994</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P46" s="1">
         <v>1</v>
@@ -3426,25 +3548,28 @@
       <c r="R46" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:18">
+      <c r="S46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="1">
         <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>23</v>
+        <v>153</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="G47" s="1">
         <v>20110510</v>
@@ -3458,7 +3583,7 @@
       <c r="J47" s="10">
         <v>838</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47" s="18">
         <v>54.7</v>
       </c>
       <c r="L47" s="1">
@@ -3471,7 +3596,7 @@
         <v>526.78800000000001</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P47" s="1">
         <v>1</v>
@@ -3482,25 +3607,28 @@
       <c r="R47" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:18">
+      <c r="S47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="1">
         <v>30</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>173</v>
+        <v>15</v>
       </c>
       <c r="G48" s="1">
         <v>20110511</v>
@@ -3514,7 +3642,7 @@
       <c r="J48" s="10">
         <v>838</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="18">
         <v>54.7</v>
       </c>
       <c r="L48" s="1">
@@ -3527,7 +3655,7 @@
         <v>516.221</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P48" s="1">
         <v>1</v>
@@ -3538,25 +3666,28 @@
       <c r="R48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:18">
+      <c r="S48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="1">
         <v>34</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="9" t="s">
-        <v>180</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
       <c r="G49" s="1">
         <v>20110511</v>
@@ -3570,7 +3701,7 @@
       <c r="J49" s="10">
         <v>838</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K49" s="18">
         <v>54.7</v>
       </c>
       <c r="L49" s="1">
@@ -3583,7 +3714,7 @@
         <v>550.49800000000005</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P49" s="1">
         <v>1</v>
@@ -3594,25 +3725,28 @@
       <c r="R49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:18">
+      <c r="S49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="1">
         <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>176</v>
+        <v>18</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>177</v>
+        <v>19</v>
       </c>
       <c r="G50" s="1">
         <v>20110512</v>
@@ -3626,7 +3760,7 @@
       <c r="J50" s="10">
         <v>838</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K50" s="18">
         <v>54.7</v>
       </c>
       <c r="L50" s="1">
@@ -3639,7 +3773,7 @@
         <v>536.69000000000005</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P50" s="1">
         <v>1</v>
@@ -3650,25 +3784,28 @@
       <c r="R50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:18">
+      <c r="S50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="1">
         <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>174</v>
+        <v>16</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>175</v>
+        <v>17</v>
       </c>
       <c r="G51" s="1">
         <v>20110513</v>
@@ -3682,7 +3819,7 @@
       <c r="J51" s="10">
         <v>200</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K51" s="18">
         <v>54.7</v>
       </c>
       <c r="L51" s="1">
@@ -3695,7 +3832,7 @@
         <v>611.78700000000003</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P51" s="1">
         <v>1</v>
@@ -3706,25 +3843,28 @@
       <c r="R51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:18">
+      <c r="S51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="1">
         <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E52" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="9" t="s">
-        <v>178</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>179</v>
+        <v>21</v>
       </c>
       <c r="G52" s="1">
         <v>20110513</v>
@@ -3738,7 +3878,7 @@
       <c r="J52" s="10">
         <v>200</v>
       </c>
-      <c r="K52" s="1">
+      <c r="K52" s="18">
         <v>54.7</v>
       </c>
       <c r="L52" s="1">
@@ -3751,7 +3891,7 @@
         <v>763.05399999999997</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="P52" s="1">
         <v>1</v>
@@ -3762,25 +3902,28 @@
       <c r="R52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:18">
+      <c r="S52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="1">
         <v>35</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>22</v>
+        <v>152</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>73</v>
+        <v>203</v>
       </c>
       <c r="G53" s="1">
         <v>20110513</v>
@@ -3794,7 +3937,7 @@
       <c r="J53" s="10">
         <v>200</v>
       </c>
-      <c r="K53" s="1">
+      <c r="K53" s="18">
         <v>54.7</v>
       </c>
       <c r="L53" s="1">
@@ -3807,7 +3950,7 @@
         <v>598.1</v>
       </c>
       <c r="O53" s="13" t="s">
-        <v>75</v>
+        <v>205</v>
       </c>
       <c r="P53" s="1">
         <v>0</v>
@@ -3818,25 +3961,28 @@
       <c r="R53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:18">
+      <c r="S53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="1">
         <v>37</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>23</v>
+        <v>153</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>74</v>
+        <v>204</v>
       </c>
       <c r="G54" s="5">
         <v>20110513</v>
@@ -3850,7 +3996,7 @@
       <c r="J54" s="10">
         <v>200</v>
       </c>
-      <c r="K54" s="1">
+      <c r="K54" s="18">
         <v>54.7</v>
       </c>
       <c r="L54" s="1">
@@ -3863,7 +4009,7 @@
         <v>584.1</v>
       </c>
       <c r="O54" s="13" t="s">
-        <v>75</v>
+        <v>205</v>
       </c>
       <c r="P54" s="1">
         <v>0</v>
@@ -3874,25 +4020,28 @@
       <c r="R54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:18">
+      <c r="S54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="1">
         <v>43</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>76</v>
+        <v>206</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>161</v>
+        <v>81</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="G55" s="5">
         <v>20110613</v>
@@ -3906,7 +4055,7 @@
       <c r="J55" s="1">
         <v>838</v>
       </c>
-      <c r="K55" s="1">
+      <c r="K55" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -3920,7 +4069,7 @@
         <v>602.95399999999995</v>
       </c>
       <c r="O55" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P55" s="1">
         <v>0</v>
@@ -3931,25 +4080,28 @@
       <c r="R55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:18">
+      <c r="S55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="1">
         <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>77</v>
+        <v>207</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G56" s="5">
         <v>20110930</v>
@@ -3963,7 +4115,7 @@
       <c r="J56" s="10">
         <v>2000</v>
       </c>
-      <c r="K56" s="1">
+      <c r="K56" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -3977,7 +4129,7 @@
         <v>659.58500000000004</v>
       </c>
       <c r="O56" s="12" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="P56" s="1">
         <v>0</v>
@@ -3988,25 +4140,28 @@
       <c r="R56" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:18">
+      <c r="S56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="1">
         <v>50</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>196</v>
+        <v>36</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>197</v>
+        <v>37</v>
       </c>
       <c r="G57" s="1">
         <v>20130423</v>
@@ -4020,7 +4175,7 @@
       <c r="J57" s="1">
         <v>838</v>
       </c>
-      <c r="K57" s="1">
+      <c r="K57" s="18">
         <v>54.7</v>
       </c>
       <c r="L57" s="1">
@@ -4033,7 +4188,7 @@
         <v>480</v>
       </c>
       <c r="O57" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P57" s="1">
         <v>0</v>
@@ -4044,25 +4199,28 @@
       <c r="R57" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:18">
+      <c r="S57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" s="1">
         <v>47</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>168</v>
+        <v>10</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>191</v>
+        <v>31</v>
       </c>
       <c r="G58" s="1">
         <v>20130627</v>
@@ -4076,7 +4234,7 @@
       <c r="J58" s="1">
         <v>838</v>
       </c>
-      <c r="K58" s="1">
+      <c r="K58" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -4090,7 +4248,7 @@
         <v>555.56799999999998</v>
       </c>
       <c r="O58" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P58" s="1">
         <v>0</v>
@@ -4101,25 +4259,28 @@
       <c r="R58" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:18">
+      <c r="S58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" s="1">
         <v>48</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>192</v>
+        <v>32</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>193</v>
+        <v>33</v>
       </c>
       <c r="G59" s="1">
         <v>20130627</v>
@@ -4133,7 +4294,7 @@
       <c r="J59" s="1">
         <v>838</v>
       </c>
-      <c r="K59" s="1">
+      <c r="K59" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -4147,7 +4308,7 @@
         <v>492.767</v>
       </c>
       <c r="O59" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P59" s="1">
         <v>0</v>
@@ -4158,25 +4319,28 @@
       <c r="R59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:18">
+      <c r="S59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60" s="1">
         <v>49</v>
       </c>
       <c r="B60" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="G60" s="1">
         <v>20130628</v>
@@ -4190,7 +4354,7 @@
       <c r="J60" s="1">
         <v>838</v>
       </c>
-      <c r="K60" s="1">
+      <c r="K60" s="18">
         <v>0</v>
       </c>
       <c r="L60" s="1">
@@ -4203,7 +4367,7 @@
         <v>540.20000000000005</v>
       </c>
       <c r="O60" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P60" s="1">
         <v>0</v>
@@ -4214,25 +4378,28 @@
       <c r="R60" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:18">
+      <c r="S60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" s="1">
         <v>51</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>198</v>
+        <v>38</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>199</v>
+        <v>39</v>
       </c>
       <c r="G61" s="1">
         <v>20130703</v>
@@ -4246,7 +4413,7 @@
       <c r="J61" s="1">
         <v>838</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K61" s="18">
         <v>54.7</v>
       </c>
       <c r="L61" s="1">
@@ -4259,7 +4426,7 @@
         <v>614.49199999999996</v>
       </c>
       <c r="O61" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P61" s="1">
         <v>0</v>
@@ -4270,25 +4437,28 @@
       <c r="R61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:18">
+      <c r="S61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" s="1">
         <v>52</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>201</v>
+        <v>41</v>
       </c>
       <c r="G62" s="1">
         <v>20130705</v>
@@ -4302,7 +4472,7 @@
       <c r="J62" s="1">
         <v>838</v>
       </c>
-      <c r="K62" s="1">
+      <c r="K62" s="18">
         <v>0</v>
       </c>
       <c r="L62" s="1">
@@ -4315,7 +4485,7 @@
         <v>578.38499999999999</v>
       </c>
       <c r="O62" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P62" s="1">
         <v>0</v>
@@ -4326,25 +4496,28 @@
       <c r="R62" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:18">
+      <c r="S62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19">
       <c r="A63" s="1">
         <v>53</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="G63" s="1">
         <v>20130827</v>
@@ -4358,7 +4531,7 @@
       <c r="J63" s="1">
         <v>838</v>
       </c>
-      <c r="K63" s="1">
+      <c r="K63" s="18">
         <v>0</v>
       </c>
       <c r="L63" s="1">
@@ -4371,7 +4544,7 @@
         <v>525.91099999999994</v>
       </c>
       <c r="O63" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P63" s="1">
         <v>0</v>
@@ -4382,25 +4555,28 @@
       <c r="R63" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:18">
+      <c r="S63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" s="1">
         <v>55</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>205</v>
+        <v>3</v>
       </c>
       <c r="G64" s="1">
         <v>20130830</v>
@@ -4414,20 +4590,20 @@
       <c r="J64" s="1">
         <v>838</v>
       </c>
-      <c r="K64" s="1" t="s">
-        <v>3</v>
+      <c r="K64" s="18" t="s">
+        <v>133</v>
       </c>
       <c r="L64" s="1">
         <v>999</v>
       </c>
       <c r="M64" s="17">
-        <v>1014.07</v>
+        <v>414.4</v>
       </c>
       <c r="N64" s="17">
-        <v>291.84899999999999</v>
+        <v>287.10000000000002</v>
       </c>
       <c r="O64" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P64" s="1">
         <v>0</v>
@@ -4438,25 +4614,28 @@
       <c r="R64" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:18">
+      <c r="S64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19">
       <c r="A65" s="1">
         <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>185</v>
+        <v>27</v>
       </c>
       <c r="G65" s="1">
         <v>20131014</v>
@@ -4470,7 +4649,7 @@
       <c r="J65" s="1">
         <v>838</v>
       </c>
-      <c r="K65" s="1">
+      <c r="K65" s="18">
         <v>0</v>
       </c>
       <c r="L65" s="1">
@@ -4483,7 +4662,7 @@
         <v>612.20000000000005</v>
       </c>
       <c r="O65" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P65" s="1">
         <v>0</v>
@@ -4494,25 +4673,28 @@
       <c r="R65" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:18">
+      <c r="S65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66" s="1">
         <v>58</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>77</v>
+        <v>207</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>156</v>
+        <v>76</v>
       </c>
       <c r="G66" s="1">
         <v>20131016</v>
@@ -4526,7 +4708,7 @@
       <c r="J66" s="1">
         <v>838</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K66" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -4540,7 +4722,7 @@
         <v>372.16199999999998</v>
       </c>
       <c r="O66" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P66" s="1">
         <v>0</v>
@@ -4551,25 +4733,28 @@
       <c r="R66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:18">
+      <c r="S66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19">
       <c r="A67" s="1">
         <v>57</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>71</v>
+        <v>201</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>184</v>
+        <v>26</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="G67" s="1">
         <v>20131108</v>
@@ -4583,7 +4768,7 @@
       <c r="J67" s="1">
         <v>838</v>
       </c>
-      <c r="K67" s="1">
+      <c r="K67" s="18">
         <f>ATAN(3)*180/PI()</f>
         <v>71.56505117707799</v>
       </c>
@@ -4597,7 +4782,7 @@
         <v>502.38200000000001</v>
       </c>
       <c r="O67" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P67" s="1">
         <v>0</v>
@@ -4608,25 +4793,28 @@
       <c r="R67" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:18">
+      <c r="S67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19">
       <c r="A68" s="1">
         <v>60</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>24</v>
+        <v>154</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>187</v>
+        <v>29</v>
       </c>
       <c r="G68" s="1">
         <v>20131202</v>
@@ -4640,7 +4828,7 @@
       <c r="J68" s="1">
         <v>838</v>
       </c>
-      <c r="K68" s="1">
+      <c r="K68" s="18">
         <v>0</v>
       </c>
       <c r="L68" s="1">
@@ -4653,7 +4841,7 @@
         <v>461.04</v>
       </c>
       <c r="O68" s="12" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="P68" s="1">
         <v>0</v>
@@ -4664,25 +4852,28 @@
       <c r="R68" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:18">
+      <c r="S68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
       <c r="A69" s="1">
         <v>59</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>189</v>
+        <v>4</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>186</v>
+        <v>28</v>
       </c>
       <c r="G69" s="1">
         <v>20131203</v>
@@ -4696,7 +4887,7 @@
       <c r="J69" s="1">
         <v>838</v>
       </c>
-      <c r="K69" s="1">
+      <c r="K69" s="18">
         <v>54.7</v>
       </c>
       <c r="L69" s="1">
@@ -4709,7 +4900,7 @@
         <v>566.50300000000004</v>
       </c>
       <c r="O69" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P69" s="1">
         <v>0</v>
@@ -4720,25 +4911,28 @@
       <c r="R69" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:18">
+      <c r="S69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
       <c r="A70" s="1">
         <v>61</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>190</v>
+        <v>5</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>188</v>
+        <v>30</v>
       </c>
       <c r="G70" s="1">
         <v>20140113</v>
@@ -4752,7 +4946,7 @@
       <c r="J70" s="1">
         <v>838</v>
       </c>
-      <c r="K70" s="1">
+      <c r="K70" s="18">
         <v>54.7</v>
       </c>
       <c r="L70" s="1">
@@ -4765,7 +4959,7 @@
         <v>477.20699999999999</v>
       </c>
       <c r="O70" s="12" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="P70" s="1">
         <v>0</v>
@@ -4776,53 +4970,56 @@
       <c r="R70" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:18">
+      <c r="S70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19">
       <c r="E71" s="9"/>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:19">
       <c r="E72" s="9"/>
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:19">
       <c r="E73" s="9"/>
       <c r="H73" s="11"/>
       <c r="I73" s="11"/>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:19">
       <c r="E74" s="9"/>
       <c r="H74" s="11"/>
       <c r="I74" s="11"/>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:19">
       <c r="E75" s="9"/>
       <c r="H75" s="11"/>
       <c r="I75" s="11"/>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:19">
       <c r="E76" s="9"/>
       <c r="H76" s="11"/>
       <c r="I76" s="11"/>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:19">
       <c r="E77" s="9"/>
       <c r="H77" s="11"/>
       <c r="I77" s="11"/>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:19">
       <c r="E78" s="9"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11"/>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:19">
       <c r="E79" s="9"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:19">
       <c r="E80" s="9"/>
       <c r="H80" s="11"/>
       <c r="I80" s="11"/>

</xml_diff>

<commit_message>
overhaul the handling of result log and its inputs and outputs
</commit_message>
<xml_diff>
--- a/mSPAGHETI_analysis_log_2014b.xlsx
+++ b/mSPAGHETI_analysis_log_2014b.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36160" yWindow="600" windowWidth="35900" windowHeight="20400" tabRatio="500"/>
+    <workbookView xWindow="-37160" yWindow="640" windowWidth="35900" windowHeight="20400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" r:id="rId1"/>
@@ -21,396 +21,36 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="208">
   <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130827_mir/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/sim_grate/A6I_scattered/scattered/</t>
-  </si>
-  <si>
-    <t>scattered-</t>
-  </si>
-  <si>
-    <t>mask200um_top10um_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131203/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20140113/SIGRTUTIShell_JHK_B/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All data present</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/G02_optical/</t>
-  </si>
-  <si>
-    <t>G02_R3_d15mm_w632nm_f838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G03/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_E_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_F/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_F_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A/</t>
-  </si>
-  <si>
-    <t>TJ07_A_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A_f200mm/</t>
-  </si>
-  <si>
-    <t>TJ07_A_d6mm_f200mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B/</t>
-  </si>
-  <si>
-    <t>TJ07_B_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B_f200mm/</t>
-  </si>
-  <si>
-    <t>TJ07_B_d6mm_f200mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C/</t>
-  </si>
-  <si>
-    <t>TJ07_C_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C_f200mm/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131016/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20131108/</t>
-  </si>
-  <si>
-    <t>mirror_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>JHKishell_d5mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>Mirror_d5mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>JHKishell_d5mm_L632_f838_B-</t>
-  </si>
-  <si>
-    <t>G03_R3_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G05/</t>
-  </si>
-  <si>
-    <t>G05_R3_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130628_mir/</t>
-  </si>
-  <si>
-    <t>mir_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130423_ishell_JHK/</t>
-  </si>
-  <si>
-    <t>ishell_JHK_JPL_wafer_R1p4_d6mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130703/</t>
-  </si>
-  <si>
-    <t>ishellJHK_d6mm_L632_f838_R1p4-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130705_mir/</t>
-  </si>
-  <si>
-    <t>mir_d6mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D_f200mm/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100217/</t>
-  </si>
-  <si>
-    <t>G1_L632nm_f400mm_d15mm_R2-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100220/</t>
-  </si>
-  <si>
-    <t>G1_L543nm_f400mm_d15mm_R2-</t>
-  </si>
-  <si>
-    <t>E06_632nm_25mm_2000mm_hdr-</t>
-  </si>
-  <si>
-    <t>TJ03F_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_G/</t>
-  </si>
-  <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ03G_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_H/</t>
-  </si>
-  <si>
-    <t>TJ03H_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110215/</t>
-  </si>
-  <si>
-    <t>TJ03E_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110217_mir/</t>
-  </si>
-  <si>
-    <t>mirror_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_G/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_G_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_H/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_H_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_I/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_I_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>TJ04_25um_J_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_A/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_A_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_B/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_B_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_C/</t>
-  </si>
-  <si>
-    <t>E09_R3_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>E12_R3_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100626/</t>
-  </si>
-  <si>
-    <t>E06_632nm_20mm_838mm_hdr-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E10/E10/</t>
-  </si>
-  <si>
-    <t>E10_20mm_632nm_838mm_R3-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E11/20110613/</t>
-  </si>
-  <si>
-    <t>E11_R3_d25mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/20110111/</t>
-  </si>
-  <si>
-    <t>g02_angle_pos1_dither1-</t>
-  </si>
-  <si>
-    <t>g02_angle_pos2_dither1-</t>
-  </si>
-  <si>
-    <t>All data present, "G" instead of "D" as suffix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JHK_JPL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/MIT/UTN18/20110131/</t>
-  </si>
-  <si>
-    <t>utn18_f838_L632_d15mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110509/</t>
-  </si>
-  <si>
-    <t>E09_R3_d25mm_f838mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110510/</t>
-  </si>
-  <si>
-    <t>E09_m0_d20mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dithered, see notes in .ppt document</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Author:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gully</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Date:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ04_100um_C_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_D/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_D_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_E/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20110930/</t>
-  </si>
-  <si>
-    <t>E12_D25mm_f2m_l632nm_R3-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101028/</t>
-  </si>
-  <si>
-    <t>JPL01_A100um_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>mir_D12_5mm_L632nm_F838mm_dith-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101102/</t>
-  </si>
-  <si>
-    <t>TJ01B_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/mir/</t>
-  </si>
-  <si>
-    <t>mir_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101103/</t>
-  </si>
-  <si>
-    <t>TJ02B_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101107/</t>
-  </si>
-  <si>
-    <t>TJ02A_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110211/</t>
-  </si>
-  <si>
-    <t>TJ03_blaze_d8_2mm_l632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213/</t>
-  </si>
-  <si>
-    <t>TJ03A_blaze_d8_2mm_l632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_C/</t>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_J/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ07_C_6mm_f200mm_632nm_sat_filt-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ07_D_6mm_f200mm_632nm_sat_filt-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a few saturated and unsaturated frames</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TJ03C_blaze_d8_2mm_l632nm-</t>
@@ -721,49 +361,408 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_J/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E09</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ07</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ07_C_6mm_f200mm_632nm_sat_filt-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ07_D_6mm_f200mm_632nm_sat_filt-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a few saturated and unsaturated frames</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E10/E10/</t>
+  </si>
+  <si>
+    <t>E10_20mm_632nm_838mm_R3-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E11/20110613/</t>
+  </si>
+  <si>
+    <t>E11_R3_d25mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/20110111/</t>
+  </si>
+  <si>
+    <t>g02_angle_pos1_dither1-</t>
+  </si>
+  <si>
+    <t>g02_angle_pos2_dither1-</t>
+  </si>
+  <si>
+    <t>All data present, "G" instead of "D" as suffix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JHK_JPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/MIT/UTN18/20110131/</t>
+  </si>
+  <si>
+    <t>utn18_f838_L632_d15mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110509/</t>
+  </si>
+  <si>
+    <t>E09_R3_d25mm_f838mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110510/</t>
+  </si>
+  <si>
+    <t>E09_m0_d20mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dithered, see notes in .ppt document</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Author:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gully</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Date:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ04_100um_C_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_D/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_D_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_E/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20110930/</t>
+  </si>
+  <si>
+    <t>E12_D25mm_f2m_l632nm_R3-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101028/</t>
+  </si>
+  <si>
+    <t>JPL01_A100um_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>mir_D12_5mm_L632nm_F838mm_dith-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101102/</t>
+  </si>
+  <si>
+    <t>TJ01B_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/mir/</t>
+  </si>
+  <si>
+    <t>mir_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101103/</t>
+  </si>
+  <si>
+    <t>TJ02B_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101107/</t>
+  </si>
+  <si>
+    <t>TJ02A_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110211/</t>
+  </si>
+  <si>
+    <t>TJ03_blaze_d8_2mm_l632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213/</t>
+  </si>
+  <si>
+    <t>TJ03A_blaze_d8_2mm_l632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_C/</t>
+  </si>
+  <si>
+    <t>ishell_JHK_JPL_wafer_R1p4_d6mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130703/</t>
+  </si>
+  <si>
+    <t>ishellJHK_d6mm_L632_f838_R1p4-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130705_mir/</t>
+  </si>
+  <si>
+    <t>mir_d6mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D_f200mm/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100217/</t>
+  </si>
+  <si>
+    <t>G1_L632nm_f400mm_d15mm_R2-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100220/</t>
+  </si>
+  <si>
+    <t>G1_L543nm_f400mm_d15mm_R2-</t>
+  </si>
+  <si>
+    <t>E06_632nm_25mm_2000mm_hdr-</t>
+  </si>
+  <si>
+    <t>TJ03F_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_G/</t>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ03G_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_H/</t>
+  </si>
+  <si>
+    <t>TJ03H_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110215/</t>
+  </si>
+  <si>
+    <t>TJ03E_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110217_mir/</t>
+  </si>
+  <si>
+    <t>mirror_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_G/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_G_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_H/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_H_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_I/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_I_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>TJ04_25um_J_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_A/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_A_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_B/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_B_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_C/</t>
+  </si>
+  <si>
+    <t>E09_R3_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>E12_R3_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100626/</t>
+  </si>
+  <si>
+    <t>E06_632nm_20mm_838mm_hdr-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130827_mir/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/sim_grate/A6I_scattered/scattered/</t>
+  </si>
+  <si>
+    <t>scattered-</t>
+  </si>
+  <si>
+    <t>mask200um_top10um_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131203/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20140113/SIGRTUTIShell_JHK_B/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All data present</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/G02_optical/</t>
+  </si>
+  <si>
+    <t>G02_R3_d15mm_w632nm_f838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G03/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_E_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_F/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_F_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A/</t>
+  </si>
+  <si>
+    <t>TJ07_A_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A_f200mm/</t>
+  </si>
+  <si>
+    <t>TJ07_A_d6mm_f200mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B/</t>
+  </si>
+  <si>
+    <t>TJ07_B_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B_f200mm/</t>
+  </si>
+  <si>
+    <t>TJ07_B_d6mm_f200mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C/</t>
+  </si>
+  <si>
+    <t>TJ07_C_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C_f200mm/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131016/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20131108/</t>
+  </si>
+  <si>
+    <t>mirror_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>JHKishell_d5mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>Mirror_d5mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>JHKishell_d5mm_L632_f838_B-</t>
+  </si>
+  <si>
+    <t>G03_R3_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G05/</t>
+  </si>
+  <si>
+    <t>G05_R3_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130628_mir/</t>
+  </si>
+  <si>
+    <t>mir_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130423_ishell_JHK/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -840,7 +839,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -850,8 +849,8 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="150" workbookViewId="0">
+      <selection activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1197,8 +1196,7 @@
     <col min="7" max="7" width="10.7109375" style="1"/>
     <col min="8" max="8" width="6" style="1" customWidth="1"/>
     <col min="9" max="10" width="5.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="4.5703125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="5.85546875" style="1" customWidth="1"/>
     <col min="13" max="14" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="6.7109375" style="1" customWidth="1"/>
@@ -1210,15 +1208,15 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2">
         <v>40190</v>
@@ -1226,140 +1224,140 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>157</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>159</v>
+        <v>43</v>
       </c>
       <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="14" t="s">
-        <v>160</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>162</v>
+        <v>46</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>138</v>
+        <v>22</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>139</v>
+        <v>23</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>164</v>
+        <v>48</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>142</v>
+        <v>26</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>144</v>
+        <v>28</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>145</v>
+        <v>29</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>146</v>
+        <v>30</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>7</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="6" t="s">
-        <v>147</v>
+        <v>31</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>166</v>
+        <v>50</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>167</v>
+        <v>51</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>168</v>
+        <v>52</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>167</v>
+        <v>51</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>169</v>
+        <v>53</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>170</v>
+        <v>54</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>171</v>
+        <v>55</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>171</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1367,19 +1365,19 @@
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>172</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>174</v>
+        <v>58</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>43</v>
+        <v>135</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="G10" s="5">
         <v>20100217</v>
@@ -1407,7 +1405,7 @@
         <v>445.50299999999999</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P10" s="1">
         <v>1</v>
@@ -1427,19 +1425,19 @@
         <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>172</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>174</v>
+        <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>46</v>
+        <v>138</v>
       </c>
       <c r="G11" s="5">
         <v>20100220</v>
@@ -1467,7 +1465,7 @@
         <v>485.83199999999999</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P11" s="1">
         <v>1</v>
@@ -1487,19 +1485,19 @@
         <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>176</v>
+        <v>60</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>177</v>
+        <v>61</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="G12" s="5">
         <v>20100624</v>
@@ -1527,7 +1525,7 @@
         <v>431.52600000000001</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P12" s="1">
         <v>1</v>
@@ -1547,19 +1545,19 @@
         <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>176</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>77</v>
+        <v>169</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>78</v>
+        <v>170</v>
       </c>
       <c r="G13" s="5">
         <v>20100626</v>
@@ -1587,7 +1585,7 @@
         <v>291.541</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P13" s="1">
         <v>1</v>
@@ -1607,19 +1605,19 @@
         <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>9</v>
+        <v>180</v>
       </c>
       <c r="G14" s="1">
         <v>20100719</v>
@@ -1647,7 +1645,7 @@
         <v>426.42599999999999</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P14" s="1">
         <v>1</v>
@@ -1667,34 +1665,34 @@
         <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>179</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>180</v>
+        <v>64</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>1</v>
+        <v>172</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2</v>
+        <v>173</v>
       </c>
       <c r="G15" s="1">
         <v>20100817</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>181</v>
+        <v>65</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>182</v>
+        <v>66</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>148</v>
+        <v>32</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="L15" s="1">
         <v>500</v>
@@ -1706,7 +1704,7 @@
         <v>707.85699999999997</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>183</v>
+        <v>67</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
@@ -1726,19 +1724,19 @@
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>184</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G16" s="5">
         <v>20100824</v>
@@ -1766,7 +1764,7 @@
         <v>390.601</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P16" s="1">
         <v>1</v>
@@ -1786,19 +1784,19 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>186</v>
+        <v>70</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>187</v>
+        <v>71</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G17" s="5">
         <v>20101028</v>
@@ -1825,7 +1823,7 @@
         <v>691.86699999999996</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P17" s="1">
         <v>1</v>
@@ -1845,19 +1843,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G18" s="5">
         <v>20101028</v>
@@ -1884,7 +1882,7 @@
         <v>258.77300000000002</v>
       </c>
       <c r="O18" s="13" t="s">
-        <v>189</v>
+        <v>73</v>
       </c>
       <c r="P18" s="1">
         <v>0</v>
@@ -1904,19 +1902,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>190</v>
+        <v>74</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G19" s="5">
         <v>20101102</v>
@@ -1943,7 +1941,7 @@
         <v>280.85700000000003</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P19" s="1">
         <v>1</v>
@@ -1963,19 +1961,19 @@
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="G20" s="5">
         <v>20101102</v>
@@ -2002,7 +2000,7 @@
         <v>357.26400000000001</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P20" s="1">
         <v>1</v>
@@ -2022,19 +2020,19 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>191</v>
+        <v>75</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G21" s="5">
         <v>20101103</v>
@@ -2061,7 +2059,7 @@
         <v>540.12099999999998</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P21" s="1">
         <v>1</v>
@@ -2081,19 +2079,19 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>191</v>
+        <v>75</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>151</v>
+        <v>35</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G22" s="5">
         <v>20101107</v>
@@ -2140,34 +2138,34 @@
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>192</v>
+        <v>76</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G23" s="5">
         <v>20110111</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="L23" s="1">
         <v>13</v>
@@ -2179,7 +2177,7 @@
         <v>662.71199999999999</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
@@ -2199,34 +2197,34 @@
         <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>193</v>
+        <v>77</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G24" s="5">
         <v>20110111</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="L24" s="1">
         <v>13</v>
@@ -2238,7 +2236,7 @@
         <v>550.70600000000002</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -2258,19 +2256,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>194</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>195</v>
+        <v>79</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="G25" s="1">
         <v>20110131</v>
@@ -2297,7 +2295,7 @@
         <v>450.29700000000003</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P25" s="1">
         <v>0</v>
@@ -2317,19 +2315,19 @@
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G26" s="5">
         <v>20110211</v>
@@ -2356,7 +2354,7 @@
         <v>519.428</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P26" s="1">
         <v>1</v>
@@ -2376,19 +2374,19 @@
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>151</v>
+        <v>35</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="G27" s="5">
         <v>20110213</v>
@@ -2415,7 +2413,7 @@
         <v>474.51</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P27" s="1">
         <v>1</v>
@@ -2435,19 +2433,19 @@
         <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>152</v>
+        <v>36</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>124</v>
+        <v>8</v>
       </c>
       <c r="G28" s="5">
         <v>20110213</v>
@@ -2474,7 +2472,7 @@
         <v>540.74300000000005</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P28" s="1">
         <v>1</v>
@@ -2494,19 +2492,19 @@
         <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>125</v>
+        <v>9</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="G29" s="5">
         <v>20110213</v>
@@ -2533,7 +2531,7 @@
         <v>446.55</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P29" s="1">
         <v>1</v>
@@ -2553,19 +2551,19 @@
         <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>49</v>
+        <v>141</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>127</v>
+        <v>11</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
       <c r="G30" s="5">
         <v>20110214</v>
@@ -2592,7 +2590,7 @@
         <v>696.42200000000003</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P30" s="1">
         <v>1</v>
@@ -2612,19 +2610,19 @@
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>51</v>
+        <v>143</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>50</v>
+        <v>142</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="G31" s="1">
         <v>20110214</v>
@@ -2651,7 +2649,7 @@
         <v>630.096</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P31" s="1">
         <v>1</v>
@@ -2671,19 +2669,19 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>56</v>
+        <v>148</v>
       </c>
       <c r="G32" s="1">
         <v>20110214</v>
@@ -2710,7 +2708,7 @@
         <v>617.91200000000003</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P32" s="1">
         <v>1</v>
@@ -2730,19 +2728,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>58</v>
+        <v>150</v>
       </c>
       <c r="G33" s="1">
         <v>20110215</v>
@@ -2769,7 +2767,7 @@
         <v>491.77600000000001</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P33" s="1">
         <v>1</v>
@@ -2789,19 +2787,19 @@
         <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="G34" s="1">
         <v>20110217</v>
@@ -2828,7 +2826,7 @@
         <v>339.34199999999998</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P34" s="1">
         <v>1</v>
@@ -2848,19 +2846,19 @@
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>51</v>
+        <v>143</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>62</v>
+        <v>154</v>
       </c>
       <c r="G35" s="1">
         <v>20110218</v>
@@ -2887,7 +2885,7 @@
         <v>758.31799999999998</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P35" s="1">
         <v>1</v>
@@ -2907,19 +2905,19 @@
         <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>64</v>
+        <v>156</v>
       </c>
       <c r="G36" s="1">
         <v>20110218</v>
@@ -2946,7 +2944,7 @@
         <v>742.60199999999998</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P36" s="1">
         <v>1</v>
@@ -2966,19 +2964,19 @@
         <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>67</v>
+        <v>159</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
       <c r="G37" s="1">
         <v>20110218</v>
@@ -3005,7 +3003,7 @@
         <v>735.83799999999997</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P37" s="1">
         <v>1</v>
@@ -3025,19 +3023,19 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>66</v>
+        <v>158</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>69</v>
+        <v>161</v>
       </c>
       <c r="G38" s="1">
         <v>20110218</v>
@@ -3064,7 +3062,7 @@
         <v>738.21199999999999</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P38" s="1">
         <v>1</v>
@@ -3084,19 +3082,19 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>151</v>
+        <v>35</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>70</v>
+        <v>162</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>71</v>
+        <v>163</v>
       </c>
       <c r="G39" s="1">
         <v>20110219</v>
@@ -3123,7 +3121,7 @@
         <v>448.11599999999999</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P39" s="1">
         <v>1</v>
@@ -3143,19 +3141,19 @@
         <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>72</v>
+        <v>164</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="G40" s="1">
         <v>20110219</v>
@@ -3182,7 +3180,7 @@
         <v>170.98699999999999</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P40" s="1">
         <v>1</v>
@@ -3202,19 +3200,19 @@
         <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>152</v>
+        <v>36</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>74</v>
+        <v>166</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G41" s="1">
         <v>20110219</v>
@@ -3241,7 +3239,7 @@
         <v>456.57</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P41" s="1">
         <v>1</v>
@@ -3261,19 +3259,19 @@
         <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="G42" s="1">
         <v>20110219</v>
@@ -3300,7 +3298,7 @@
         <v>339.42599999999999</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P42" s="1">
         <v>1</v>
@@ -3320,19 +3318,19 @@
         <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="G43" s="1">
         <v>20110219</v>
@@ -3359,7 +3357,7 @@
         <v>191.54900000000001</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P43" s="1">
         <v>1</v>
@@ -3379,19 +3377,19 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>49</v>
+        <v>141</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>12</v>
+        <v>183</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="G44" s="1">
         <v>20110219</v>
@@ -3418,7 +3416,7 @@
         <v>470.45100000000002</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P44" s="1">
         <v>1</v>
@@ -3438,19 +3436,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>201</v>
+        <v>1</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G45" s="1">
         <v>20110509</v>
@@ -3478,7 +3476,7 @@
         <v>629.98099999999999</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P45" s="1">
         <v>1</v>
@@ -3498,19 +3496,19 @@
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>201</v>
+        <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G46" s="5">
         <v>20110510</v>
@@ -3537,7 +3535,7 @@
         <v>535.78599999999994</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P46" s="1">
         <v>1</v>
@@ -3557,19 +3555,19 @@
         <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>129</v>
+        <v>13</v>
       </c>
       <c r="G47" s="1">
         <v>20110510</v>
@@ -3596,7 +3594,7 @@
         <v>526.78800000000001</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P47" s="1">
         <v>1</v>
@@ -3616,19 +3614,19 @@
         <v>30</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E48" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>14</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
       <c r="G48" s="1">
         <v>20110511</v>
@@ -3655,7 +3653,7 @@
         <v>516.221</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P48" s="1">
         <v>1</v>
@@ -3675,19 +3673,19 @@
         <v>34</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>152</v>
+        <v>36</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>22</v>
+        <v>193</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>23</v>
+        <v>194</v>
       </c>
       <c r="G49" s="1">
         <v>20110511</v>
@@ -3714,7 +3712,7 @@
         <v>550.49800000000005</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P49" s="1">
         <v>1</v>
@@ -3734,19 +3732,19 @@
         <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>19</v>
+        <v>190</v>
       </c>
       <c r="G50" s="1">
         <v>20110512</v>
@@ -3773,7 +3771,7 @@
         <v>536.69000000000005</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P50" s="1">
         <v>1</v>
@@ -3793,19 +3791,19 @@
         <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>151</v>
+        <v>35</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>16</v>
+        <v>187</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="G51" s="1">
         <v>20110513</v>
@@ -3832,7 +3830,7 @@
         <v>611.78700000000003</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P51" s="1">
         <v>1</v>
@@ -3852,19 +3850,19 @@
         <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>20</v>
+        <v>191</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>21</v>
+        <v>192</v>
       </c>
       <c r="G52" s="1">
         <v>20110513</v>
@@ -3891,7 +3889,7 @@
         <v>763.05399999999997</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="P52" s="1">
         <v>1</v>
@@ -3911,19 +3909,19 @@
         <v>35</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>152</v>
+        <v>36</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>24</v>
+        <v>195</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>203</v>
+        <v>3</v>
       </c>
       <c r="G53" s="1">
         <v>20110513</v>
@@ -3950,7 +3948,7 @@
         <v>598.1</v>
       </c>
       <c r="O53" s="13" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
       <c r="P53" s="1">
         <v>0</v>
@@ -3970,19 +3968,19 @@
         <v>37</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>204</v>
+        <v>4</v>
       </c>
       <c r="G54" s="5">
         <v>20110513</v>
@@ -4009,7 +4007,7 @@
         <v>584.1</v>
       </c>
       <c r="O54" s="13" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
       <c r="P54" s="1">
         <v>0</v>
@@ -4029,19 +4027,19 @@
         <v>43</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>206</v>
+        <v>6</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G55" s="5">
         <v>20110613</v>
@@ -4069,7 +4067,7 @@
         <v>602.95399999999995</v>
       </c>
       <c r="O55" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P55" s="1">
         <v>0</v>
@@ -4089,19 +4087,19 @@
         <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>207</v>
+        <v>7</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G56" s="5">
         <v>20110930</v>
@@ -4129,7 +4127,7 @@
         <v>659.58500000000004</v>
       </c>
       <c r="O56" s="12" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="P56" s="1">
         <v>0</v>
@@ -4149,19 +4147,19 @@
         <v>50</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="G57" s="1">
         <v>20130423</v>
@@ -4188,7 +4186,7 @@
         <v>480</v>
       </c>
       <c r="O57" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P57" s="1">
         <v>0</v>
@@ -4208,19 +4206,19 @@
         <v>47</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>31</v>
+        <v>202</v>
       </c>
       <c r="G58" s="1">
         <v>20130627</v>
@@ -4248,7 +4246,7 @@
         <v>555.56799999999998</v>
       </c>
       <c r="O58" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P58" s="1">
         <v>0</v>
@@ -4268,19 +4266,19 @@
         <v>48</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>33</v>
+        <v>204</v>
       </c>
       <c r="G59" s="1">
         <v>20130627</v>
@@ -4308,7 +4306,7 @@
         <v>492.767</v>
       </c>
       <c r="O59" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P59" s="1">
         <v>0</v>
@@ -4328,19 +4326,19 @@
         <v>49</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>34</v>
+        <v>205</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>35</v>
+        <v>206</v>
       </c>
       <c r="G60" s="1">
         <v>20130628</v>
@@ -4367,7 +4365,7 @@
         <v>540.20000000000005</v>
       </c>
       <c r="O60" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P60" s="1">
         <v>0</v>
@@ -4387,19 +4385,19 @@
         <v>51</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>198</v>
+        <v>82</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="F61" s="1" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="G61" s="1">
         <v>20130703</v>
@@ -4426,7 +4424,7 @@
         <v>614.49199999999996</v>
       </c>
       <c r="O61" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P61" s="1">
         <v>0</v>
@@ -4446,19 +4444,19 @@
         <v>52</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="G62" s="1">
         <v>20130705</v>
@@ -4485,7 +4483,7 @@
         <v>578.38499999999999</v>
       </c>
       <c r="O62" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P62" s="1">
         <v>0</v>
@@ -4505,19 +4503,19 @@
         <v>53</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>35</v>
+        <v>206</v>
       </c>
       <c r="G63" s="1">
         <v>20130827</v>
@@ -4544,7 +4542,7 @@
         <v>525.91099999999994</v>
       </c>
       <c r="O63" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P63" s="1">
         <v>0</v>
@@ -4564,19 +4562,19 @@
         <v>55</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>131</v>
+        <v>15</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>3</v>
+        <v>174</v>
       </c>
       <c r="G64" s="1">
         <v>20130830</v>
@@ -4591,7 +4589,7 @@
         <v>838</v>
       </c>
       <c r="K64" s="18" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="L64" s="1">
         <v>999</v>
@@ -4603,7 +4601,7 @@
         <v>287.10000000000002</v>
       </c>
       <c r="O64" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P64" s="1">
         <v>0</v>
@@ -4623,19 +4621,19 @@
         <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>27</v>
+        <v>198</v>
       </c>
       <c r="G65" s="1">
         <v>20131014</v>
@@ -4662,7 +4660,7 @@
         <v>612.20000000000005</v>
       </c>
       <c r="O65" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P65" s="1">
         <v>0</v>
@@ -4682,19 +4680,19 @@
         <v>58</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>207</v>
+        <v>7</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>25</v>
+        <v>196</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>76</v>
+        <v>168</v>
       </c>
       <c r="G66" s="1">
         <v>20131016</v>
@@ -4722,7 +4720,7 @@
         <v>372.16199999999998</v>
       </c>
       <c r="O66" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P66" s="1">
         <v>0</v>
@@ -4742,19 +4740,19 @@
         <v>57</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>201</v>
+        <v>1</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>26</v>
+        <v>197</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c r="G67" s="1">
         <v>20131108</v>
@@ -4782,7 +4780,7 @@
         <v>502.38200000000001</v>
       </c>
       <c r="O67" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P67" s="1">
         <v>0</v>
@@ -4802,19 +4800,19 @@
         <v>60</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>29</v>
+        <v>200</v>
       </c>
       <c r="G68" s="1">
         <v>20131202</v>
@@ -4841,7 +4839,7 @@
         <v>461.04</v>
       </c>
       <c r="O68" s="12" t="s">
-        <v>6</v>
+        <v>177</v>
       </c>
       <c r="P68" s="1">
         <v>0</v>
@@ -4861,19 +4859,19 @@
         <v>59</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>151</v>
+        <v>35</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>4</v>
+        <v>175</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>28</v>
+        <v>199</v>
       </c>
       <c r="G69" s="1">
         <v>20131203</v>
@@ -4900,7 +4898,7 @@
         <v>566.50300000000004</v>
       </c>
       <c r="O69" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P69" s="1">
         <v>0</v>
@@ -4920,19 +4918,19 @@
         <v>61</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>30</v>
+        <v>201</v>
       </c>
       <c r="G70" s="1">
         <v>20140113</v>
@@ -4959,7 +4957,7 @@
         <v>477.20699999999999</v>
       </c>
       <c r="O70" s="12" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="P70" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
minor tweaks, I think
</commit_message>
<xml_diff>
--- a/mSPAGHETI_analysis_log_2014b.xlsx
+++ b/mSPAGHETI_analysis_log_2014b.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37160" yWindow="640" windowWidth="35900" windowHeight="20400" tabRatio="500"/>
+    <workbookView xWindow="-36840" yWindow="2820" windowWidth="33620" windowHeight="18600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,454 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="208">
   <si>
+    <t>G03_R3_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G05/</t>
+  </si>
+  <si>
+    <t>G05_R3_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130628_mir/</t>
+  </si>
+  <si>
+    <t>mir_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130423_ishell_JHK/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_B/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_B_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_C/</t>
+  </si>
+  <si>
+    <t>E09_R3_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>E12_R3_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100626/</t>
+  </si>
+  <si>
+    <t>E06_632nm_20mm_838mm_hdr-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130827_mir/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/sim_grate/A6I_scattered/scattered/</t>
+  </si>
+  <si>
+    <t>scattered-</t>
+  </si>
+  <si>
+    <t>mask200um_top10um_d25mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131203/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20140113/SIGRTUTIShell_JHK_B/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All data present</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/G02_optical/</t>
+  </si>
+  <si>
+    <t>G02_R3_d15mm_w632nm_f838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G03/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_E_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_F/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_F_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A/</t>
+  </si>
+  <si>
+    <t>TJ07_A_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A_f200mm/</t>
+  </si>
+  <si>
+    <t>TJ07_A_d6mm_f200mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B/</t>
+  </si>
+  <si>
+    <t>TJ07_B_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B_f200mm/</t>
+  </si>
+  <si>
+    <t>TJ07_B_d6mm_f200mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C/</t>
+  </si>
+  <si>
+    <t>TJ07_C_d6mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C_f200mm/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131016/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20131108/</t>
+  </si>
+  <si>
+    <t>mirror_d15mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>JHKishell_d5mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>Mirror_d5mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>JHKishell_d5mm_L632_f838_B-</t>
+  </si>
+  <si>
+    <t>TJ02A_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110211/</t>
+  </si>
+  <si>
+    <t>TJ03_blaze_d8_2mm_l632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213/</t>
+  </si>
+  <si>
+    <t>TJ03A_blaze_d8_2mm_l632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_C/</t>
+  </si>
+  <si>
+    <t>ishell_JHK_JPL_wafer_R1p4_d6mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130703/</t>
+  </si>
+  <si>
+    <t>ishellJHK_d6mm_L632_f838_R1p4-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130705_mir/</t>
+  </si>
+  <si>
+    <t>mir_d6mm_L632_f838-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D_f200mm/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100217/</t>
+  </si>
+  <si>
+    <t>G1_L632nm_f400mm_d15mm_R2-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100220/</t>
+  </si>
+  <si>
+    <t>G1_L543nm_f400mm_d15mm_R2-</t>
+  </si>
+  <si>
+    <t>E06_632nm_25mm_2000mm_hdr-</t>
+  </si>
+  <si>
+    <t>TJ03F_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_G/</t>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ03G_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_H/</t>
+  </si>
+  <si>
+    <t>TJ03H_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110215/</t>
+  </si>
+  <si>
+    <t>TJ03E_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110217_mir/</t>
+  </si>
+  <si>
+    <t>mirror_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_G/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_G_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_H/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_H_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_I/</t>
+  </si>
+  <si>
+    <t>TJ04_25um_I_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>TJ04_25um_J_blaze_d8_2mm_l632nm_FL200mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_A/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_A_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>JPL01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A100um</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mirror</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dithered</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>utn18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All data present</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E10/E10/</t>
+  </si>
+  <si>
+    <t>E10_20mm_632nm_838mm_R3-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E11/20110613/</t>
+  </si>
+  <si>
+    <t>E11_R3_d25mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/20110111/</t>
+  </si>
+  <si>
+    <t>g02_angle_pos1_dither1-</t>
+  </si>
+  <si>
+    <t>g02_angle_pos2_dither1-</t>
+  </si>
+  <si>
+    <t>All data present, "G" instead of "D" as suffix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JHK_JPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/MIT/UTN18/20110131/</t>
+  </si>
+  <si>
+    <t>utn18_f838_L632_d15mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110509/</t>
+  </si>
+  <si>
+    <t>E09_R3_d25mm_f838mm_632nm_filt-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110510/</t>
+  </si>
+  <si>
+    <t>E09_m0_d20mm_f838mm_632nm-</t>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dithered, see notes in .ppt document</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Author:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gully</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Date:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TJ04_100um_C_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_D/</t>
+  </si>
+  <si>
+    <t>TJ04_100um_D_blaze_d8_2mm_l632nm_FL838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_E/</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20110930/</t>
+  </si>
+  <si>
+    <t>E12_D25mm_f2m_l632nm_R3-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101028/</t>
+  </si>
+  <si>
+    <t>JPL01_A100um_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>mir_D12_5mm_L632nm_F838mm_dith-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101102/</t>
+  </si>
+  <si>
+    <t>TJ01B_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/mir/</t>
+  </si>
+  <si>
+    <t>mir_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101103/</t>
+  </si>
+  <si>
+    <t>TJ02B_D12_5mm_L632nm_F838mm-</t>
+  </si>
+  <si>
+    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101107/</t>
+  </si>
+  <si>
     <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_J/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -304,454 +752,6 @@
     <t>JPL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>JPL01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A100um</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mirror</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dithered</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pos1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pos2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>utn18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All data present</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JPL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E10/E10/</t>
-  </si>
-  <si>
-    <t>E10_20mm_632nm_838mm_R3-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E11/20110613/</t>
-  </si>
-  <si>
-    <t>E11_R3_d25mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/20110111/</t>
-  </si>
-  <si>
-    <t>g02_angle_pos1_dither1-</t>
-  </si>
-  <si>
-    <t>g02_angle_pos2_dither1-</t>
-  </si>
-  <si>
-    <t>All data present, "G" instead of "D" as suffix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JHK_JPL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/MIT/UTN18/20110131/</t>
-  </si>
-  <si>
-    <t>utn18_f838_L632_d15mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110509/</t>
-  </si>
-  <si>
-    <t>E09_R3_d25mm_f838mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20110510/</t>
-  </si>
-  <si>
-    <t>E09_m0_d20mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dithered, see notes in .ppt document</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Author:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gully</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Date:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ04_100um_C_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_D/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_D_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_E/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20110930/</t>
-  </si>
-  <si>
-    <t>E12_D25mm_f2m_l632nm_R3-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101028/</t>
-  </si>
-  <si>
-    <t>JPL01_A100um_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>mir_D12_5mm_L632nm_F838mm_dith-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/20101102/</t>
-  </si>
-  <si>
-    <t>TJ01B_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL01/mir/</t>
-  </si>
-  <si>
-    <t>mir_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101103/</t>
-  </si>
-  <si>
-    <t>TJ02B_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/JPL02/20101107/</t>
-  </si>
-  <si>
-    <t>TJ02A_D12_5mm_L632nm_F838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110211/</t>
-  </si>
-  <si>
-    <t>TJ03_blaze_d8_2mm_l632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213/</t>
-  </si>
-  <si>
-    <t>TJ03A_blaze_d8_2mm_l632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110213_C/</t>
-  </si>
-  <si>
-    <t>ishell_JHK_JPL_wafer_R1p4_d6mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130703/</t>
-  </si>
-  <si>
-    <t>ishellJHK_d6mm_L632_f838_R1p4-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130705_mir/</t>
-  </si>
-  <si>
-    <t>mir_d6mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/D_f200mm/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100217/</t>
-  </si>
-  <si>
-    <t>G1_L632nm_f400mm_d15mm_R2-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Heritage/G1/20100220/</t>
-  </si>
-  <si>
-    <t>G1_L543nm_f400mm_d15mm_R2-</t>
-  </si>
-  <si>
-    <t>E06_632nm_25mm_2000mm_hdr-</t>
-  </si>
-  <si>
-    <t>TJ03F_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_G/</t>
-  </si>
-  <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TJ03G_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110214_H/</t>
-  </si>
-  <si>
-    <t>TJ03H_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ03/20110215/</t>
-  </si>
-  <si>
-    <t>TJ03E_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110217_mir/</t>
-  </si>
-  <si>
-    <t>mirror_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_G/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_G_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_H/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_H_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110218_I/</t>
-  </si>
-  <si>
-    <t>TJ04_25um_I_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>TJ04_25um_J_blaze_d8_2mm_l632nm_FL200mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_A/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_A_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_B/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_B_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_C/</t>
-  </si>
-  <si>
-    <t>E09_R3_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>E12_R3_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/E06/20100626/</t>
-  </si>
-  <si>
-    <t>E06_632nm_20mm_838mm_hdr-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/Processing_exposure/masks/pitch200um_top10um_1995mask/20130827_mir/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/sim_grate/A6I_scattered/scattered/</t>
-  </si>
-  <si>
-    <t>scattered-</t>
-  </si>
-  <si>
-    <t>mask200um_top10um_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20131203/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20140113/SIGRTUTIShell_JHK_B/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All data present</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G02/G02_optical/</t>
-  </si>
-  <si>
-    <t>G02_R3_d15mm_w632nm_f838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G03/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_E_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ04/20110219_F/</t>
-  </si>
-  <si>
-    <t>TJ04_100um_F_blaze_d8_2mm_l632nm_FL838mm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A/</t>
-  </si>
-  <si>
-    <t>TJ07_A_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/A_f200mm/</t>
-  </si>
-  <si>
-    <t>TJ07_A_d6mm_f200mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B/</t>
-  </si>
-  <si>
-    <t>TJ07_B_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/B_f200mm/</t>
-  </si>
-  <si>
-    <t>TJ07_B_d6mm_f200mm_632nm_filt-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C/</t>
-  </si>
-  <si>
-    <t>TJ07_C_d6mm_f838mm_632nm-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/TJ07/C_f200mm/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E12/20131016/</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/APRA_JPL/E09/20131108/</t>
-  </si>
-  <si>
-    <t>mirror_d15mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>JHKishell_d5mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>Mirror_d5mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>JHKishell_d5mm_L632_f838_B-</t>
-  </si>
-  <si>
-    <t>G03_R3_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130627_G05/</t>
-  </si>
-  <si>
-    <t>G05_R3_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/G05/HeNe_632/20130628_mir/</t>
-  </si>
-  <si>
-    <t>mir_d25mm_L632_f838-</t>
-  </si>
-  <si>
-    <t>/Volumes/cambridge/Astronomy/silicon/iShell/JHK_grating/spectral_purity/20130423_ishell_JHK/</t>
-  </si>
 </sst>
 </file>
 
@@ -762,7 +762,7 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -839,7 +839,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -849,8 +849,8 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1182,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="150" workbookViewId="0">
-      <selection activeCell="L76" sqref="L76"/>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1208,15 +1208,15 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="B2" s="2">
         <v>40190</v>
@@ -1224,140 +1224,140 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>43</v>
+        <v>181</v>
       </c>
       <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="14" t="s">
-        <v>44</v>
+        <v>182</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>184</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="S7" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="S7" s="15" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>169</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>51</v>
+        <v>189</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>52</v>
+        <v>190</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>51</v>
+        <v>189</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>53</v>
+        <v>191</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>55</v>
+        <v>193</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>55</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1365,19 +1365,19 @@
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>135</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="G10" s="5">
         <v>20100217</v>
@@ -1405,7 +1405,7 @@
         <v>445.50299999999999</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P10" s="1">
         <v>1</v>
@@ -1425,19 +1425,19 @@
         <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>137</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="G11" s="5">
         <v>20100220</v>
@@ -1465,7 +1465,7 @@
         <v>485.83199999999999</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P11" s="1">
         <v>1</v>
@@ -1485,19 +1485,19 @@
         <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="G12" s="5">
         <v>20100624</v>
@@ -1525,7 +1525,7 @@
         <v>431.52600000000001</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P12" s="1">
         <v>1</v>
@@ -1545,19 +1545,19 @@
         <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>198</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="G13" s="5">
         <v>20100626</v>
@@ -1585,7 +1585,7 @@
         <v>291.541</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P13" s="1">
         <v>1</v>
@@ -1605,19 +1605,19 @@
         <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>200</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>179</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>180</v>
+        <v>22</v>
       </c>
       <c r="G14" s="1">
         <v>20100719</v>
@@ -1645,7 +1645,7 @@
         <v>426.42599999999999</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P14" s="1">
         <v>1</v>
@@ -1665,34 +1665,34 @@
         <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>202</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>173</v>
+        <v>15</v>
       </c>
       <c r="G15" s="1">
         <v>20100817</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>65</v>
+        <v>203</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>32</v>
+        <v>170</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="L15" s="1">
         <v>500</v>
@@ -1704,7 +1704,7 @@
         <v>707.85699999999997</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>67</v>
+        <v>205</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
@@ -1724,19 +1724,19 @@
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>206</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5">
         <v>20100824</v>
@@ -1764,7 +1764,7 @@
         <v>390.601</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P16" s="1">
         <v>1</v>
@@ -1784,19 +1784,19 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="G17" s="5">
         <v>20101028</v>
@@ -1823,7 +1823,7 @@
         <v>691.86699999999996</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P17" s="1">
         <v>1</v>
@@ -1843,19 +1843,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="G18" s="5">
         <v>20101028</v>
@@ -1882,7 +1882,7 @@
         <v>258.77300000000002</v>
       </c>
       <c r="O18" s="13" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="P18" s="1">
         <v>0</v>
@@ -1902,19 +1902,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="G19" s="5">
         <v>20101102</v>
@@ -1941,7 +1941,7 @@
         <v>280.85700000000003</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P19" s="1">
         <v>1</v>
@@ -1961,19 +1961,19 @@
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="G20" s="5">
         <v>20101102</v>
@@ -2000,7 +2000,7 @@
         <v>357.26400000000001</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P20" s="1">
         <v>1</v>
@@ -2020,19 +2020,19 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="G21" s="5">
         <v>20101103</v>
@@ -2059,7 +2059,7 @@
         <v>540.12099999999998</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P21" s="1">
         <v>1</v>
@@ -2079,19 +2079,19 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="G22" s="5">
         <v>20101107</v>
@@ -2138,34 +2138,34 @@
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>200</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="G23" s="5">
         <v>20110111</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="L23" s="1">
         <v>13</v>
@@ -2177,7 +2177,7 @@
         <v>662.71199999999999</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
@@ -2197,34 +2197,34 @@
         <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>200</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="G24" s="5">
         <v>20110111</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="L24" s="1">
         <v>13</v>
@@ -2236,7 +2236,7 @@
         <v>550.70600000000002</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -2256,19 +2256,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="G25" s="1">
         <v>20110131</v>
@@ -2295,7 +2295,7 @@
         <v>450.29700000000003</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P25" s="1">
         <v>0</v>
@@ -2315,19 +2315,19 @@
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="G26" s="5">
         <v>20110211</v>
@@ -2354,7 +2354,7 @@
         <v>519.428</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P26" s="1">
         <v>1</v>
@@ -2374,19 +2374,19 @@
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="G27" s="5">
         <v>20110213</v>
@@ -2413,7 +2413,7 @@
         <v>474.51</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P27" s="1">
         <v>1</v>
@@ -2433,19 +2433,19 @@
         <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
+        <v>174</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>128</v>
+        <v>49</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>8</v>
+        <v>146</v>
       </c>
       <c r="G28" s="5">
         <v>20110213</v>
@@ -2472,7 +2472,7 @@
         <v>540.74300000000005</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P28" s="1">
         <v>1</v>
@@ -2492,19 +2492,19 @@
         <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>9</v>
+        <v>147</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>10</v>
+        <v>148</v>
       </c>
       <c r="G29" s="5">
         <v>20110213</v>
@@ -2531,7 +2531,7 @@
         <v>446.55</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P29" s="1">
         <v>1</v>
@@ -2551,19 +2551,19 @@
         <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>141</v>
+        <v>62</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>11</v>
+        <v>149</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>140</v>
+        <v>61</v>
       </c>
       <c r="G30" s="5">
         <v>20110214</v>
@@ -2590,7 +2590,7 @@
         <v>696.42200000000003</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P30" s="1">
         <v>1</v>
@@ -2610,19 +2610,19 @@
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>143</v>
+        <v>64</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>142</v>
+        <v>63</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>146</v>
+        <v>67</v>
       </c>
       <c r="G31" s="1">
         <v>20110214</v>
@@ -2649,7 +2649,7 @@
         <v>630.096</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P31" s="1">
         <v>1</v>
@@ -2669,19 +2669,19 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="G32" s="1">
         <v>20110214</v>
@@ -2708,7 +2708,7 @@
         <v>617.91200000000003</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P32" s="1">
         <v>1</v>
@@ -2728,19 +2728,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>149</v>
+        <v>70</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>150</v>
+        <v>71</v>
       </c>
       <c r="G33" s="1">
         <v>20110215</v>
@@ -2767,7 +2767,7 @@
         <v>491.77600000000001</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P33" s="1">
         <v>1</v>
@@ -2787,19 +2787,19 @@
         <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>152</v>
+        <v>73</v>
       </c>
       <c r="G34" s="1">
         <v>20110217</v>
@@ -2826,7 +2826,7 @@
         <v>339.34199999999998</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P34" s="1">
         <v>1</v>
@@ -2846,19 +2846,19 @@
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>143</v>
+        <v>64</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>154</v>
+        <v>75</v>
       </c>
       <c r="G35" s="1">
         <v>20110218</v>
@@ -2885,7 +2885,7 @@
         <v>758.31799999999998</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P35" s="1">
         <v>1</v>
@@ -2905,19 +2905,19 @@
         <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>156</v>
+        <v>77</v>
       </c>
       <c r="G36" s="1">
         <v>20110218</v>
@@ -2944,7 +2944,7 @@
         <v>742.60199999999998</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P36" s="1">
         <v>1</v>
@@ -2964,19 +2964,19 @@
         <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>157</v>
+        <v>78</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
       <c r="G37" s="1">
         <v>20110218</v>
@@ -3003,7 +3003,7 @@
         <v>735.83799999999997</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P37" s="1">
         <v>1</v>
@@ -3023,19 +3023,19 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>161</v>
+        <v>82</v>
       </c>
       <c r="G38" s="1">
         <v>20110218</v>
@@ -3062,7 +3062,7 @@
         <v>738.21199999999999</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P38" s="1">
         <v>1</v>
@@ -3082,19 +3082,19 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>163</v>
+        <v>84</v>
       </c>
       <c r="G39" s="1">
         <v>20110219</v>
@@ -3121,7 +3121,7 @@
         <v>448.11599999999999</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P39" s="1">
         <v>1</v>
@@ -3141,19 +3141,19 @@
         <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>164</v>
+        <v>6</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="G40" s="1">
         <v>20110219</v>
@@ -3180,7 +3180,7 @@
         <v>170.98699999999999</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P40" s="1">
         <v>1</v>
@@ -3200,19 +3200,19 @@
         <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>36</v>
+        <v>174</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="G41" s="1">
         <v>20110219</v>
@@ -3239,7 +3239,7 @@
         <v>456.57</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P41" s="1">
         <v>1</v>
@@ -3259,19 +3259,19 @@
         <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="G42" s="1">
         <v>20110219</v>
@@ -3298,7 +3298,7 @@
         <v>339.42599999999999</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P42" s="1">
         <v>1</v>
@@ -3318,19 +3318,19 @@
         <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
       <c r="G43" s="1">
         <v>20110219</v>
@@ -3357,7 +3357,7 @@
         <v>191.54900000000001</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P43" s="1">
         <v>1</v>
@@ -3377,19 +3377,19 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>141</v>
+        <v>62</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>184</v>
+        <v>26</v>
       </c>
       <c r="G44" s="1">
         <v>20110219</v>
@@ -3416,7 +3416,7 @@
         <v>470.45100000000002</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P44" s="1">
         <v>1</v>
@@ -3436,19 +3436,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="G45" s="1">
         <v>20110509</v>
@@ -3476,7 +3476,7 @@
         <v>629.98099999999999</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P45" s="1">
         <v>1</v>
@@ -3496,19 +3496,19 @@
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="G46" s="5">
         <v>20110510</v>
@@ -3535,7 +3535,7 @@
         <v>535.78599999999994</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P46" s="1">
         <v>1</v>
@@ -3555,19 +3555,19 @@
         <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>13</v>
+        <v>151</v>
       </c>
       <c r="G47" s="1">
         <v>20110510</v>
@@ -3594,7 +3594,7 @@
         <v>526.78800000000001</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P47" s="1">
         <v>1</v>
@@ -3614,19 +3614,19 @@
         <v>30</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>185</v>
+        <v>27</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>186</v>
+        <v>28</v>
       </c>
       <c r="G48" s="1">
         <v>20110511</v>
@@ -3653,7 +3653,7 @@
         <v>516.221</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P48" s="1">
         <v>1</v>
@@ -3673,19 +3673,19 @@
         <v>34</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="G49" s="1">
         <v>20110511</v>
@@ -3712,7 +3712,7 @@
         <v>550.49800000000005</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P49" s="1">
         <v>1</v>
@@ -3732,19 +3732,19 @@
         <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>189</v>
+        <v>31</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>190</v>
+        <v>32</v>
       </c>
       <c r="G50" s="1">
         <v>20110512</v>
@@ -3771,7 +3771,7 @@
         <v>536.69000000000005</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P50" s="1">
         <v>1</v>
@@ -3791,19 +3791,19 @@
         <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>187</v>
+        <v>29</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>188</v>
+        <v>30</v>
       </c>
       <c r="G51" s="1">
         <v>20110513</v>
@@ -3830,7 +3830,7 @@
         <v>611.78700000000003</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P51" s="1">
         <v>1</v>
@@ -3850,19 +3850,19 @@
         <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="G52" s="1">
         <v>20110513</v>
@@ -3889,7 +3889,7 @@
         <v>763.05399999999997</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="P52" s="1">
         <v>1</v>
@@ -3909,19 +3909,19 @@
         <v>35</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>36</v>
+        <v>174</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>195</v>
+        <v>37</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>3</v>
+        <v>141</v>
       </c>
       <c r="G53" s="1">
         <v>20110513</v>
@@ -3948,7 +3948,7 @@
         <v>598.1</v>
       </c>
       <c r="O53" s="13" t="s">
-        <v>5</v>
+        <v>143</v>
       </c>
       <c r="P53" s="1">
         <v>0</v>
@@ -3968,19 +3968,19 @@
         <v>37</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>134</v>
+        <v>55</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="G54" s="5">
         <v>20110513</v>
@@ -4007,7 +4007,7 @@
         <v>584.1</v>
       </c>
       <c r="O54" s="13" t="s">
-        <v>5</v>
+        <v>143</v>
       </c>
       <c r="P54" s="1">
         <v>0</v>
@@ -4027,19 +4027,19 @@
         <v>43</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="G55" s="5">
         <v>20110613</v>
@@ -4067,7 +4067,7 @@
         <v>602.95399999999995</v>
       </c>
       <c r="O55" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P55" s="1">
         <v>0</v>
@@ -4087,19 +4087,19 @@
         <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="G56" s="5">
         <v>20110930</v>
@@ -4127,7 +4127,7 @@
         <v>659.58500000000004</v>
       </c>
       <c r="O56" s="12" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="P56" s="1">
         <v>0</v>
@@ -4147,19 +4147,19 @@
         <v>50</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>207</v>
+        <v>5</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>129</v>
+        <v>50</v>
       </c>
       <c r="G57" s="1">
         <v>20130423</v>
@@ -4186,7 +4186,7 @@
         <v>480</v>
       </c>
       <c r="O57" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P57" s="1">
         <v>0</v>
@@ -4206,19 +4206,19 @@
         <v>47</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="G58" s="1">
         <v>20130627</v>
@@ -4246,7 +4246,7 @@
         <v>555.56799999999998</v>
       </c>
       <c r="O58" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P58" s="1">
         <v>0</v>
@@ -4266,19 +4266,19 @@
         <v>48</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>203</v>
+        <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>204</v>
+        <v>2</v>
       </c>
       <c r="G59" s="1">
         <v>20130627</v>
@@ -4306,7 +4306,7 @@
         <v>492.767</v>
       </c>
       <c r="O59" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P59" s="1">
         <v>0</v>
@@ -4326,19 +4326,19 @@
         <v>49</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>205</v>
+        <v>3</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="G60" s="1">
         <v>20130628</v>
@@ -4365,7 +4365,7 @@
         <v>540.20000000000005</v>
       </c>
       <c r="O60" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P60" s="1">
         <v>0</v>
@@ -4385,19 +4385,19 @@
         <v>51</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>14</v>
+        <v>152</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>130</v>
+        <v>51</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="G61" s="1">
         <v>20130703</v>
@@ -4424,7 +4424,7 @@
         <v>614.49199999999996</v>
       </c>
       <c r="O61" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P61" s="1">
         <v>0</v>
@@ -4444,19 +4444,19 @@
         <v>52</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>132</v>
+        <v>53</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>133</v>
+        <v>54</v>
       </c>
       <c r="G62" s="1">
         <v>20130705</v>
@@ -4483,7 +4483,7 @@
         <v>578.38499999999999</v>
       </c>
       <c r="O62" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P62" s="1">
         <v>0</v>
@@ -4503,19 +4503,19 @@
         <v>53</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="G63" s="1">
         <v>20130827</v>
@@ -4542,7 +4542,7 @@
         <v>525.91099999999994</v>
       </c>
       <c r="O63" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P63" s="1">
         <v>0</v>
@@ -4562,19 +4562,19 @@
         <v>55</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>15</v>
+        <v>153</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E64" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="G64" s="1">
         <v>20130830</v>
@@ -4589,7 +4589,7 @@
         <v>838</v>
       </c>
       <c r="K64" s="18" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
       <c r="L64" s="1">
         <v>999</v>
@@ -4601,7 +4601,7 @@
         <v>287.10000000000002</v>
       </c>
       <c r="O64" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P64" s="1">
         <v>0</v>
@@ -4621,19 +4621,19 @@
         <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>198</v>
+        <v>40</v>
       </c>
       <c r="G65" s="1">
         <v>20131014</v>
@@ -4660,7 +4660,7 @@
         <v>612.20000000000005</v>
       </c>
       <c r="O65" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P65" s="1">
         <v>0</v>
@@ -4680,19 +4680,19 @@
         <v>58</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>196</v>
+        <v>38</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>168</v>
+        <v>10</v>
       </c>
       <c r="G66" s="1">
         <v>20131016</v>
@@ -4720,7 +4720,7 @@
         <v>372.16199999999998</v>
       </c>
       <c r="O66" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P66" s="1">
         <v>0</v>
@@ -4740,19 +4740,19 @@
         <v>57</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>197</v>
+        <v>39</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>167</v>
+        <v>9</v>
       </c>
       <c r="G67" s="1">
         <v>20131108</v>
@@ -4780,7 +4780,7 @@
         <v>502.38200000000001</v>
       </c>
       <c r="O67" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P67" s="1">
         <v>0</v>
@@ -4800,19 +4800,19 @@
         <v>60</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>38</v>
+        <v>176</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>200</v>
+        <v>42</v>
       </c>
       <c r="G68" s="1">
         <v>20131202</v>
@@ -4839,7 +4839,7 @@
         <v>461.04</v>
       </c>
       <c r="O68" s="12" t="s">
-        <v>177</v>
+        <v>19</v>
       </c>
       <c r="P68" s="1">
         <v>0</v>
@@ -4859,19 +4859,19 @@
         <v>59</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>175</v>
+        <v>17</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>199</v>
+        <v>41</v>
       </c>
       <c r="G69" s="1">
         <v>20131203</v>
@@ -4898,7 +4898,7 @@
         <v>566.50300000000004</v>
       </c>
       <c r="O69" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P69" s="1">
         <v>0</v>
@@ -4918,19 +4918,19 @@
         <v>61</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>176</v>
+        <v>18</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>201</v>
+        <v>43</v>
       </c>
       <c r="G70" s="1">
         <v>20140113</v>
@@ -4957,7 +4957,7 @@
         <v>477.20699999999999</v>
       </c>
       <c r="O70" s="12" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P70" s="1">
         <v>0</v>

</xml_diff>